<commit_message>
Added new commands to regression testing
</commit_message>
<xml_diff>
--- a/Resources/testdata/TestData.xlsx
+++ b/Resources/testdata/TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="299">
   <si>
     <t>Info</t>
   </si>
@@ -918,13 +918,16 @@
   </si>
   <si>
     <t>YL EID Power</t>
+  </si>
+  <si>
+    <t>MC DEV EUI Power</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -955,6 +958,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF66FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -975,7 +985,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -998,13 +1008,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1019,6 +1040,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1557,7 +1581,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2565,7 +2589,7 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2579,6 +2603,7 @@
     <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -2612,6 +2637,9 @@
       <c r="J1" s="8" t="s">
         <v>297</v>
       </c>
+      <c r="K1" s="10" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2638,14 +2666,14 @@
       <c r="H2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>142</v>
+      <c r="I2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2673,14 +2701,14 @@
       <c r="H3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>148</v>
+      <c r="I3" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2708,14 +2736,14 @@
       <c r="H4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>182</v>
+      <c r="I4" s="12" t="s">
+        <v>168</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>154</v>
+        <v>169</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2743,14 +2771,14 @@
       <c r="H5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>188</v>
+      <c r="I5" s="12" t="s">
+        <v>182</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>153</v>
+        <v>183</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2778,14 +2806,14 @@
       <c r="H6" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>289</v>
+      <c r="I6" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>189</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2813,14 +2841,14 @@
       <c r="H7" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>282</v>
+      <c r="I7" s="11" t="s">
+        <v>288</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2848,14 +2876,14 @@
       <c r="H8" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>196</v>
+      <c r="I8" s="11" t="s">
+        <v>282</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>172</v>
+        <v>283</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2883,14 +2911,14 @@
       <c r="H9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>198</v>
+      <c r="I9" s="11" t="s">
+        <v>196</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>178</v>
+        <v>197</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2918,14 +2946,14 @@
       <c r="H10" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>202</v>
+      <c r="I10" s="11" t="s">
+        <v>198</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>161</v>
+        <v>199</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2953,14 +2981,14 @@
       <c r="H11" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="I11" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>175</v>
+      <c r="I11" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>203</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2976,14 +3004,14 @@
       <c r="D12" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="I12" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>190</v>
+      <c r="I12" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2999,14 +3027,14 @@
       <c r="D13" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="I13" s="3" t="s">
-        <v>290</v>
+      <c r="I13" s="11" t="s">
+        <v>278</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>194</v>
+        <v>279</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3022,14 +3050,14 @@
       <c r="D14" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="I14" s="3" t="s">
-        <v>210</v>
+      <c r="I14" s="11" t="s">
+        <v>290</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>165</v>
+        <v>291</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3045,14 +3073,14 @@
       <c r="D15" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="I15" s="3" t="s">
-        <v>248</v>
+      <c r="I15" s="11" t="s">
+        <v>210</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>249</v>
+        <v>211</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>200</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3068,14 +3096,14 @@
       <c r="D16" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="I16" s="3" t="s">
-        <v>286</v>
+      <c r="I16" s="11" t="s">
+        <v>248</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>171</v>
+        <v>249</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -3091,14 +3119,14 @@
       <c r="D17" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="I17" s="3" t="s">
-        <v>292</v>
+      <c r="I17" s="11" t="s">
+        <v>286</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -3114,14 +3142,14 @@
       <c r="D18" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="I18" s="3" t="s">
-        <v>206</v>
+      <c r="I18" s="11" t="s">
+        <v>292</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>207</v>
+        <v>293</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -3137,14 +3165,14 @@
       <c r="D19" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>242</v>
+      <c r="I19" s="11" t="s">
+        <v>206</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -3160,14 +3188,14 @@
       <c r="D20" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>232</v>
+      <c r="I20" s="11" t="s">
+        <v>242</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>216</v>
+        <v>243</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -3183,14 +3211,14 @@
       <c r="D21" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>258</v>
+      <c r="I21" s="11" t="s">
+        <v>232</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>218</v>
+        <v>233</v>
+      </c>
+      <c r="K21" s="11" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -3207,13 +3235,13 @@
         <v>221</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>222</v>
+        <v>259</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -3229,14 +3257,14 @@
       <c r="D23" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I23" s="3" t="s">
-        <v>214</v>
+      <c r="I23" s="11" t="s">
+        <v>262</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>215</v>
+        <v>263</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -3252,14 +3280,14 @@
       <c r="D24" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="I24" s="3" t="s">
-        <v>220</v>
+      <c r="I24" s="11" t="s">
+        <v>214</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>228</v>
+        <v>215</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -3275,14 +3303,14 @@
       <c r="D25" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="I25" s="3" t="s">
-        <v>238</v>
+      <c r="I25" s="11" t="s">
+        <v>220</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>230</v>
+        <v>221</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -3298,14 +3326,14 @@
       <c r="D26" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="I26" s="3" t="s">
-        <v>254</v>
+      <c r="I26" s="11" t="s">
+        <v>238</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>234</v>
+        <v>239</v>
+      </c>
+      <c r="K26" s="11" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -3321,14 +3349,14 @@
       <c r="D27" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I27" s="3" t="s">
-        <v>280</v>
+      <c r="I27" s="11" t="s">
+        <v>254</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>236</v>
+        <v>255</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -3344,14 +3372,14 @@
       <c r="D28" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="I28" s="3" t="s">
-        <v>266</v>
+      <c r="I28" s="11" t="s">
+        <v>280</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>240</v>
+        <v>281</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -3367,14 +3395,14 @@
       <c r="D29" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="I29" s="3" t="s">
-        <v>204</v>
+      <c r="I29" s="11" t="s">
+        <v>266</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="K29" s="3" t="s">
-        <v>244</v>
+        <v>267</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -3390,14 +3418,14 @@
       <c r="D30" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="I30" s="3" t="s">
-        <v>284</v>
+      <c r="I30" s="11" t="s">
+        <v>204</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="K30" s="3" t="s">
-        <v>246</v>
+        <v>205</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -3413,14 +3441,14 @@
       <c r="D31" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="I31" s="3" t="s">
-        <v>192</v>
+      <c r="I31" s="11" t="s">
+        <v>284</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="K31" s="3" t="s">
-        <v>185</v>
+        <v>285</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -3436,14 +3464,14 @@
       <c r="D32" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="I32" s="3" t="s">
-        <v>250</v>
+      <c r="I32" s="11" t="s">
+        <v>192</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>251</v>
+        <v>193</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>252</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -3460,13 +3488,13 @@
         <v>255</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>256</v>
+        <v>251</v>
+      </c>
+      <c r="K33" s="11" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -3482,14 +3510,14 @@
       <c r="D34" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="I34" s="3" t="s">
-        <v>294</v>
+      <c r="I34" s="11" t="s">
+        <v>272</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="K34" s="3" t="s">
-        <v>260</v>
+        <v>273</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -3505,8 +3533,14 @@
       <c r="D35" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="K35" s="3" t="s">
-        <v>264</v>
+      <c r="I35" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K35" s="11" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -3522,8 +3556,8 @@
       <c r="D36" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="K36" s="3" t="s">
-        <v>268</v>
+      <c r="K36" s="11" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -3539,8 +3573,8 @@
       <c r="D37" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="K37" s="3" t="s">
-        <v>270</v>
+      <c r="K37" s="11" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -3556,8 +3590,8 @@
       <c r="D38" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="K38" s="3" t="s">
-        <v>274</v>
+      <c r="K38" s="11" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -3573,8 +3607,8 @@
       <c r="D39" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="K39" s="3" t="s">
-        <v>252</v>
+      <c r="K39" s="11" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -3591,7 +3625,7 @@
         <v>279</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>230</v>
+        <v>252</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -3607,7 +3641,9 @@
       <c r="D41" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="K41" s="3"/>
+      <c r="K41" s="3" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>

</xml_diff>

<commit_message>
Added daily reading script
</commit_message>
<xml_diff>
--- a/Resources/testdata/TestData.xlsx
+++ b/Resources/testdata/TestData.xlsx
@@ -9,22 +9,96 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12930" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
-    <sheet name="enviornment" sheetId="1" r:id="rId1"/>
-    <sheet name="appserver" sheetId="2" r:id="rId2"/>
-    <sheet name="devices" sheetId="3" r:id="rId3"/>
-    <sheet name="yl_command" sheetId="4" r:id="rId4"/>
-    <sheet name="yl_command_test" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
+    <sheet name="report" sheetId="1" r:id="rId1"/>
+    <sheet name="enviornment" sheetId="2" r:id="rId2"/>
+    <sheet name="appserver" sheetId="3" r:id="rId3"/>
+    <sheet name="devices" sheetId="4" r:id="rId4"/>
+    <sheet name="yl_command" sheetId="5" r:id="rId5"/>
+    <sheet name="yl_command_test" sheetId="6" r:id="rId6"/>
+    <sheet name="device info" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="320">
+  <si>
+    <t>Date
+Period</t>
+  </si>
+  <si>
+    <t>Total 
+Devices</t>
+  </si>
+  <si>
+    <t>Online 
+Devices</t>
+  </si>
+  <si>
+    <t>Device Availablilty 
+Rate</t>
+  </si>
+  <si>
+    <t>Unsolicited msg 
+not  Received</t>
+  </si>
+  <si>
+    <t>Unsolicited msg  
+Received</t>
+  </si>
+  <si>
+    <t>Unsolicited msg Received 
+Rate</t>
+  </si>
+  <si>
+    <t>Scheduled msg 
+not Reived</t>
+  </si>
+  <si>
+    <t>Scheduled msg 
+Reived</t>
+  </si>
+  <si>
+    <t>Scheduled msg 
+Rate</t>
+  </si>
+  <si>
+    <t>Devices with no data</t>
+  </si>
+  <si>
+    <t>17-09-24 ~ 17-09-25</t>
+  </si>
+  <si>
+    <t>['7ff9010202000024', '7ff9010202000026', '7ff9010202000031', '7ff9010202000032', '7ff9010202000037', '7ff9010202000084', '7ff9010202000092', '7ff9010202000095', '7ff9010202000098', '7ff9010202000108', '7ff9010202000116', '7ff9010202000153', '7ff9010202000162', '7ff9010202000163', '7ff9010202000164', '7ff9010202000166']</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>96.30%</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>66.67%</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>0.00%</t>
+  </si>
   <si>
     <t>Info</t>
   </si>
@@ -95,7 +169,7 @@
     <t>SESSION ID</t>
   </si>
   <si>
-    <t>4266c1b2c29d83b56191200553bfe826</t>
+    <t>152bcc70991a26b5ac737ab7edc5424a</t>
   </si>
   <si>
     <t>c775cf20a052fce804617cbea5266ab3</t>
@@ -143,315 +217,522 @@
     <t>AS_URL</t>
   </si>
   <si>
+    <t>000f161202000112</t>
+  </si>
+  <si>
+    <t>8000000000000001</t>
+  </si>
+  <si>
+    <t>2b7e151628aed2a6abf7158809cf4f3c</t>
+  </si>
+  <si>
+    <t>YL POW</t>
+  </si>
+  <si>
+    <t>000f161202000022</t>
+  </si>
+  <si>
+    <t>000f161202000026</t>
+  </si>
+  <si>
+    <t>000f161202000027</t>
+  </si>
+  <si>
+    <t>000f161202000162</t>
+  </si>
+  <si>
+    <t>000f161202000118</t>
+  </si>
+  <si>
+    <t>000f161202000030</t>
+  </si>
+  <si>
+    <t>000f161202000031</t>
+  </si>
+  <si>
+    <t>000f161202000032</t>
+  </si>
+  <si>
+    <t>000f161202000024</t>
+  </si>
+  <si>
+    <t>000f161202000113</t>
+  </si>
+  <si>
+    <t>000f161202000163</t>
+  </si>
+  <si>
+    <t>000f161202000081</t>
+  </si>
+  <si>
+    <t>000f161202000098</t>
+  </si>
+  <si>
+    <t>000f161202000161</t>
+  </si>
+  <si>
+    <t>000f161202000164</t>
+  </si>
+  <si>
+    <t>000f161202000037</t>
+  </si>
+  <si>
+    <t>000f161202000095</t>
+  </si>
+  <si>
+    <t>000f161202000088</t>
+  </si>
+  <si>
+    <t>000f161202000103</t>
+  </si>
+  <si>
+    <t>000f161202000104</t>
+  </si>
+  <si>
+    <t>000f161202000082</t>
+  </si>
+  <si>
+    <t>000f161202000084</t>
+  </si>
+  <si>
+    <t>000f161202000092</t>
+  </si>
+  <si>
+    <t>000f161202000102</t>
+  </si>
+  <si>
+    <t>000f161202000116</t>
+  </si>
+  <si>
+    <t>000f161202000106</t>
+  </si>
+  <si>
+    <t>000f161202000036</t>
+  </si>
+  <si>
+    <t>000f161202000153</t>
+  </si>
+  <si>
+    <t>000f161202000028</t>
+  </si>
+  <si>
+    <t>000f161202000100</t>
+  </si>
+  <si>
+    <t>000f161202000108</t>
+  </si>
+  <si>
+    <t>000f161202000166</t>
+  </si>
+  <si>
+    <t>MC EID</t>
+  </si>
+  <si>
+    <t>YL</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>7ff9010202000112</t>
+  </si>
+  <si>
+    <t>7ff9010202000025</t>
+  </si>
+  <si>
+    <t>7ff9010202000034</t>
+  </si>
+  <si>
+    <t>7ff9010202000022</t>
+  </si>
+  <si>
+    <t>7ff9010202000083</t>
+  </si>
+  <si>
+    <t>7ff9010202000035</t>
+  </si>
+  <si>
+    <t>7ff9010202000026</t>
+  </si>
+  <si>
+    <t>7ff9010202000085</t>
+  </si>
+  <si>
+    <t>7ff9010202000043</t>
+  </si>
+  <si>
+    <t>7ff9010202000027</t>
+  </si>
+  <si>
+    <t>7ff9010202000087</t>
+  </si>
+  <si>
+    <t>7ff9010202000045</t>
+  </si>
+  <si>
+    <t>7ff9010202000162</t>
+  </si>
+  <si>
+    <t>7ff9010202000090</t>
+  </si>
+  <si>
+    <t>7ff9010202000055</t>
+  </si>
+  <si>
+    <t>7ff9010202000118</t>
+  </si>
+  <si>
+    <t>7ff9010202000097</t>
+  </si>
+  <si>
+    <t>7ff9010202000059</t>
+  </si>
+  <si>
+    <t>7ff9010202000030</t>
+  </si>
+  <si>
+    <t>7ff9010202000107</t>
+  </si>
+  <si>
+    <t>7ff9010202000061</t>
+  </si>
+  <si>
+    <t>7ff9010202000031</t>
+  </si>
+  <si>
+    <t>7ff9010202000117</t>
+  </si>
+  <si>
+    <t>7ff9010202000064</t>
+  </si>
+  <si>
+    <t>7ff9010202000032</t>
+  </si>
+  <si>
+    <t>7ff9010202000165</t>
+  </si>
+  <si>
+    <t>7ff9010202000127</t>
+  </si>
+  <si>
+    <t>7ff9010202000024</t>
+  </si>
+  <si>
+    <t>7ff9010202000167</t>
+  </si>
+  <si>
+    <t>7ff9010202000137</t>
+  </si>
+  <si>
+    <t>7ff9010202000113</t>
+  </si>
+  <si>
+    <t>7ff9010202000163</t>
+  </si>
+  <si>
+    <t>7ff9010202000081</t>
+  </si>
+  <si>
+    <t>7ff9010202000098</t>
+  </si>
+  <si>
+    <t>7ff9010202000161</t>
+  </si>
+  <si>
+    <t>7ff9010202000164</t>
+  </si>
+  <si>
+    <t>7ff9010202000037</t>
+  </si>
+  <si>
+    <t>7ff9010202000095</t>
+  </si>
+  <si>
+    <t>7ff9010202000088</t>
+  </si>
+  <si>
+    <t>7ff9010202000103</t>
+  </si>
+  <si>
+    <t>7ff9010202000104</t>
+  </si>
+  <si>
+    <t>7ff9010202000082</t>
+  </si>
+  <si>
+    <t>7ff9010202000084</t>
+  </si>
+  <si>
+    <t>7ff9010202000092</t>
+  </si>
+  <si>
+    <t>7ff9010202000102</t>
+  </si>
+  <si>
+    <t>7ff9010202000116</t>
+  </si>
+  <si>
+    <t>7ff9010202000106</t>
+  </si>
+  <si>
+    <t>7ff9010202000036</t>
+  </si>
+  <si>
+    <t>7ff9010202000153</t>
+  </si>
+  <si>
+    <t>7ff9010202000028</t>
+  </si>
+  <si>
+    <t>7ff9010202000100</t>
+  </si>
+  <si>
+    <t>7ff9010202000108</t>
+  </si>
+  <si>
+    <t>7ff9010202000166</t>
+  </si>
+  <si>
+    <t>COMMAND</t>
+  </si>
+  <si>
+    <t>PARAMETER</t>
+  </si>
+  <si>
+    <t>GET_METER_TYPE</t>
+  </si>
+  <si>
+    <t>GET_METER_SUMMATION_DELIVERED</t>
+  </si>
+  <si>
+    <t>GET_METER_CURRENT_PRESSURE</t>
+  </si>
+  <si>
+    <t>SET_METER_GAS_VALVE_STATE</t>
+  </si>
+  <si>
+    <t>valve_state=1</t>
+  </si>
+  <si>
+    <t>GET_METER_GAS_VALVE_STATE</t>
+  </si>
+  <si>
+    <t>valve_state=0</t>
+  </si>
+  <si>
+    <t>SET_SUMMATION_REPORT_INTERVAL</t>
+  </si>
+  <si>
+    <t>report_interval_mins=6</t>
+  </si>
+  <si>
+    <t>GET_SUMMATION_REPORT_INTERVAL</t>
+  </si>
+  <si>
+    <t>report_interval_mins=1440</t>
+  </si>
+  <si>
+    <t>SET_PRESSURE_REPORT_INTERVAL</t>
+  </si>
+  <si>
+    <t>GET_PRESSURE_REPORT_INTERVAL</t>
+  </si>
+  <si>
+    <t>GET_METER_VERSION</t>
+  </si>
+  <si>
+    <t>SET_OFLOW_DETECT_ENABLE</t>
+  </si>
+  <si>
+    <t>overflow_detect_enable=0</t>
+  </si>
+  <si>
+    <t>GET_OFLOW_DETECT_ENABLE</t>
+  </si>
+  <si>
+    <t>overflow_detect_enable=1</t>
+  </si>
+  <si>
+    <t>SET_OFLOW_DETECT_DURATION</t>
+  </si>
+  <si>
+    <t>overflow_detect_duration=5</t>
+  </si>
+  <si>
+    <t>GET_OFLOW_DETECT_DURATION</t>
+  </si>
+  <si>
+    <t>overflow_detect_duration=999</t>
+  </si>
+  <si>
+    <t>SET_OFLOW_DETECT_RATE</t>
+  </si>
+  <si>
+    <t>overflow_detect_duration=13</t>
+  </si>
+  <si>
+    <t>GET_OFLOW_DETECT_RATE</t>
+  </si>
+  <si>
+    <t>overflow_detect_duration=40</t>
+  </si>
+  <si>
+    <t>SET_PRESSURE_ALARM_LEVEL_LOW</t>
+  </si>
+  <si>
+    <t>pressure_alarm_level_low=0</t>
+  </si>
+  <si>
+    <t>GET_PRESSURE_ALARM_LEVEL_LOW</t>
+  </si>
+  <si>
+    <t>pressure_alarm_level_low=5</t>
+  </si>
+  <si>
+    <t>SET_PRESSURE_ALARM_LEVEL_HIGH</t>
+  </si>
+  <si>
+    <t>pressure_alarm_level_high=0</t>
+  </si>
+  <si>
+    <t>GET_PRESSURE_ALARM_LEVEL_HIGH</t>
+  </si>
+  <si>
+    <t>pressure_alarm_level_high=5</t>
+  </si>
+  <si>
+    <t>SET_LEAK_DETECT_RANGE</t>
+  </si>
+  <si>
+    <t>leak_detect_range=0</t>
+  </si>
+  <si>
+    <t>GET_LEAK_DETECT_RANGE</t>
+  </si>
+  <si>
+    <t>leak_detect_range=9</t>
+  </si>
+  <si>
+    <t>SET_MANUAL_RECOVER_ENABLE</t>
+  </si>
+  <si>
+    <t>manual_recover_enable=0</t>
+  </si>
+  <si>
+    <t>GET_MANUAL_RECOVER_ENABLE</t>
+  </si>
+  <si>
+    <t>manual_recover_enable=9</t>
+  </si>
+  <si>
+    <t>GET_METER_FIRMWARE_VERSION</t>
+  </si>
+  <si>
+    <t>GET_METER_SHUTOFF_CODES</t>
+  </si>
+  <si>
+    <t>SET_METER_SERIAL_NUMBER</t>
+  </si>
+  <si>
+    <t>meter_serial_number=testchar01</t>
+  </si>
+  <si>
+    <t>GET_METER_SERIAL_NUMBER</t>
+  </si>
+  <si>
+    <t>meter_serial_number=testchar99</t>
+  </si>
+  <si>
+    <t>GET_ELECTRIC_QNT_VALUE</t>
+  </si>
+  <si>
+    <t>SET_COMMS_MODE</t>
+  </si>
+  <si>
+    <t>meter_comms_mode=0</t>
+  </si>
+  <si>
+    <t>GET_COMMS_MODE</t>
+  </si>
+  <si>
+    <t>meter_comms_mode=1</t>
+  </si>
+  <si>
+    <t>SET_PILOT_LIGHT_MODE</t>
+  </si>
+  <si>
+    <t>pilot_light_mode=0,pilot_flow_min=9,pilot_flow_max=50</t>
+  </si>
+  <si>
+    <t>GET_PILOT_LIGHT_MODE</t>
+  </si>
+  <si>
+    <t>pilot_light_mode=1,pilot_flow_min=13,pilot_flow_max=53</t>
+  </si>
+  <si>
+    <t>SET_EARTHQUAKE_SENSOR_STATE</t>
+  </si>
+  <si>
+    <t>earthquake_sensor_state=0</t>
+  </si>
+  <si>
+    <t>GET_EARTHQUAKE_SENSOR_STATE</t>
+  </si>
+  <si>
+    <t>MC DEV EUI</t>
+  </si>
+  <si>
+    <t>YL DEV EUI</t>
+  </si>
+  <si>
+    <t>YL EID</t>
+  </si>
+  <si>
+    <t>YL DEV EUI Battery</t>
+  </si>
+  <si>
+    <t>YL EID Battery</t>
+  </si>
+  <si>
+    <t>MC DEV EUI Battery</t>
+  </si>
+  <si>
+    <t>MC EID Battery</t>
+  </si>
+  <si>
+    <t>YL DEV EUI Power</t>
+  </si>
+  <si>
+    <t>YL EID Power</t>
+  </si>
+  <si>
+    <t>MC DEV EUI Power</t>
+  </si>
+  <si>
+    <t>000f161202000038</t>
+  </si>
+  <si>
+    <t>7ff9010202000038</t>
+  </si>
+  <si>
+    <t>000f161202000012</t>
+  </si>
+  <si>
+    <t>7ff9010202000012</t>
+  </si>
+  <si>
+    <t>000f161202000025</t>
+  </si>
+  <si>
+    <t>000f161202000034</t>
+  </si>
+  <si>
     <t>000f161202000016</t>
   </si>
   <si>
-    <t>8000000000000001</t>
-  </si>
-  <si>
-    <t>2b7e151628aed2a6abf7158809cf4f3c</t>
-  </si>
-  <si>
-    <t>YL POW</t>
-  </si>
-  <si>
-    <t>MC EID</t>
-  </si>
-  <si>
-    <t>YL</t>
-  </si>
-  <si>
-    <t>MC</t>
-  </si>
-  <si>
     <t>7ff9010202000016</t>
   </si>
   <si>
-    <t>7ff9010202000025</t>
-  </si>
-  <si>
-    <t>7ff9010202000034</t>
-  </si>
-  <si>
-    <t>7ff9010202000083</t>
-  </si>
-  <si>
-    <t>7ff9010202000035</t>
-  </si>
-  <si>
-    <t>7ff9010202000085</t>
-  </si>
-  <si>
-    <t>7ff9010202000043</t>
-  </si>
-  <si>
-    <t>7ff9010202000087</t>
-  </si>
-  <si>
-    <t>7ff9010202000045</t>
-  </si>
-  <si>
-    <t>7ff9010202000090</t>
-  </si>
-  <si>
-    <t>7ff9010202000055</t>
-  </si>
-  <si>
-    <t>7ff9010202000097</t>
-  </si>
-  <si>
-    <t>7ff9010202000059</t>
-  </si>
-  <si>
-    <t>7ff9010202000107</t>
-  </si>
-  <si>
-    <t>7ff9010202000061</t>
-  </si>
-  <si>
-    <t>7ff9010202000117</t>
-  </si>
-  <si>
-    <t>7ff9010202000064</t>
-  </si>
-  <si>
-    <t>7ff9010202000165</t>
-  </si>
-  <si>
-    <t>7ff9010202000127</t>
-  </si>
-  <si>
-    <t>7ff9010202000167</t>
-  </si>
-  <si>
-    <t>7ff9010202000137</t>
-  </si>
-  <si>
-    <t>COMMAND</t>
-  </si>
-  <si>
-    <t>PARAMETER</t>
-  </si>
-  <si>
-    <t>GET_METER_TYPE</t>
-  </si>
-  <si>
-    <t>GET_METER_SUMMATION_DELIVERED</t>
-  </si>
-  <si>
-    <t>GET_METER_CURRENT_PRESSURE</t>
-  </si>
-  <si>
-    <t>SET_METER_GAS_VALVE_STATE</t>
-  </si>
-  <si>
-    <t>valve_state=1</t>
-  </si>
-  <si>
-    <t>GET_METER_GAS_VALVE_STATE</t>
-  </si>
-  <si>
-    <t>valve_state=0</t>
-  </si>
-  <si>
-    <t>SET_SUMMATION_REPORT_INTERVAL</t>
-  </si>
-  <si>
-    <t>report_interval_mins=6</t>
-  </si>
-  <si>
-    <t>GET_SUMMATION_REPORT_INTERVAL</t>
-  </si>
-  <si>
-    <t>report_interval_mins=1440</t>
-  </si>
-  <si>
-    <t>SET_PRESSURE_REPORT_INTERVAL</t>
-  </si>
-  <si>
-    <t>GET_PRESSURE_REPORT_INTERVAL</t>
-  </si>
-  <si>
-    <t>GET_METER_VERSION</t>
-  </si>
-  <si>
-    <t>SET_OFLOW_DETECT_ENABLE</t>
-  </si>
-  <si>
-    <t>overflow_detect_enable=0</t>
-  </si>
-  <si>
-    <t>GET_OFLOW_DETECT_ENABLE</t>
-  </si>
-  <si>
-    <t>overflow_detect_enable=1</t>
-  </si>
-  <si>
-    <t>SET_OFLOW_DETECT_DURATION</t>
-  </si>
-  <si>
-    <t>overflow_detect_duration=5</t>
-  </si>
-  <si>
-    <t>GET_OFLOW_DETECT_DURATION</t>
-  </si>
-  <si>
-    <t>overflow_detect_duration=999</t>
-  </si>
-  <si>
-    <t>SET_OFLOW_DETECT_RATE</t>
-  </si>
-  <si>
-    <t>overflow_detect_duration=13</t>
-  </si>
-  <si>
-    <t>GET_OFLOW_DETECT_RATE</t>
-  </si>
-  <si>
-    <t>overflow_detect_duration=40</t>
-  </si>
-  <si>
-    <t>SET_PRESSURE_ALARM_LEVEL_LOW</t>
-  </si>
-  <si>
-    <t>pressure_alarm_level_low=0</t>
-  </si>
-  <si>
-    <t>GET_PRESSURE_ALARM_LEVEL_LOW</t>
-  </si>
-  <si>
-    <t>pressure_alarm_level_low=5</t>
-  </si>
-  <si>
-    <t>SET_PRESSURE_ALARM_LEVEL_HIGH</t>
-  </si>
-  <si>
-    <t>pressure_alarm_level_high=0</t>
-  </si>
-  <si>
-    <t>GET_PRESSURE_ALARM_LEVEL_HIGH</t>
-  </si>
-  <si>
-    <t>pressure_alarm_level_high=5</t>
-  </si>
-  <si>
-    <t>SET_LEAK_DETECT_RANGE</t>
-  </si>
-  <si>
-    <t>leak_detect_range=0</t>
-  </si>
-  <si>
-    <t>GET_LEAK_DETECT_RANGE</t>
-  </si>
-  <si>
-    <t>leak_detect_range=9</t>
-  </si>
-  <si>
-    <t>SET_MANUAL_RECOVER_ENABLE</t>
-  </si>
-  <si>
-    <t>manual_recover_enable=0</t>
-  </si>
-  <si>
-    <t>GET_MANUAL_RECOVER_ENABLE</t>
-  </si>
-  <si>
-    <t>manual_recover_enable=9</t>
-  </si>
-  <si>
-    <t>GET_METER_FIRMWARE_VERSION</t>
-  </si>
-  <si>
-    <t>GET_METER_SHUTOFF_CODES</t>
-  </si>
-  <si>
-    <t>SET_METER_SERIAL_NUMBER</t>
-  </si>
-  <si>
-    <t>meter_serial_number=testchar01</t>
-  </si>
-  <si>
-    <t>GET_METER_SERIAL_NUMBER</t>
-  </si>
-  <si>
-    <t>meter_serial_number=testchar99</t>
-  </si>
-  <si>
-    <t>GET_ELECTRIC_QNT_VALUE</t>
-  </si>
-  <si>
-    <t>SET_COMMS_MODE</t>
-  </si>
-  <si>
-    <t>meter_comms_mode=0</t>
-  </si>
-  <si>
-    <t>GET_COMMS_MODE</t>
-  </si>
-  <si>
-    <t>meter_comms_mode=1</t>
-  </si>
-  <si>
-    <t>SET_PILOT_LIGHT_MODE</t>
-  </si>
-  <si>
-    <t>pilot_light_mode=0,pilot_flow_min=9,pilot_flow_max=50</t>
-  </si>
-  <si>
-    <t>GET_PILOT_LIGHT_MODE</t>
-  </si>
-  <si>
-    <t>pilot_light_mode=1,pilot_flow_min=13,pilot_flow_max=53</t>
-  </si>
-  <si>
-    <t>SET_EARTHQUAKE_SENSOR_STATE</t>
-  </si>
-  <si>
-    <t>earthquake_sensor_state=0</t>
-  </si>
-  <si>
-    <t>GET_EARTHQUAKE_SENSOR_STATE</t>
-  </si>
-  <si>
-    <t>MC DEV EUI</t>
-  </si>
-  <si>
-    <t>YL DEV EUI</t>
-  </si>
-  <si>
-    <t>YL EID</t>
-  </si>
-  <si>
-    <t>YL DEV EUI Battery</t>
-  </si>
-  <si>
-    <t>YL EID Battery</t>
-  </si>
-  <si>
-    <t>MC DEV EUI Battery</t>
-  </si>
-  <si>
-    <t>MC EID Battery</t>
-  </si>
-  <si>
-    <t>000f161202000038</t>
-  </si>
-  <si>
-    <t>7ff9010202000038</t>
-  </si>
-  <si>
-    <t>000f161202000012</t>
-  </si>
-  <si>
-    <t>7ff9010202000012</t>
-  </si>
-  <si>
-    <t>000f161202000025</t>
-  </si>
-  <si>
-    <t>000f161202000034</t>
-  </si>
-  <si>
     <t>000f161202000039</t>
   </si>
   <si>
@@ -530,12 +811,6 @@
     <t>7ff9010202000049</t>
   </si>
   <si>
-    <t>000f161202000022</t>
-  </si>
-  <si>
-    <t>7ff9010202000022</t>
-  </si>
-  <si>
     <t>000f161202000107</t>
   </si>
   <si>
@@ -548,12 +823,6 @@
     <t>7ff9010202000050</t>
   </si>
   <si>
-    <t>000f161202000024</t>
-  </si>
-  <si>
-    <t>7ff9010202000024</t>
-  </si>
-  <si>
     <t>000f161202000117</t>
   </si>
   <si>
@@ -572,12 +841,6 @@
     <t>000f161202000127</t>
   </si>
   <si>
-    <t>000f161202000026</t>
-  </si>
-  <si>
-    <t>7ff9010202000026</t>
-  </si>
-  <si>
     <t>000f161202000167</t>
   </si>
   <si>
@@ -590,90 +853,36 @@
     <t>7ff9010202000056</t>
   </si>
   <si>
-    <t>000f161202000027</t>
-  </si>
-  <si>
-    <t>7ff9010202000027</t>
-  </si>
-  <si>
     <t>000f161202000057</t>
   </si>
   <si>
     <t>7ff9010202000057</t>
   </si>
   <si>
-    <t>000f161202000028</t>
-  </si>
-  <si>
-    <t>7ff9010202000028</t>
-  </si>
-  <si>
     <t>000f161202000058</t>
   </si>
   <si>
     <t>7ff9010202000058</t>
   </si>
   <si>
-    <t>000f161202000030</t>
-  </si>
-  <si>
-    <t>7ff9010202000030</t>
-  </si>
-  <si>
-    <t>000f161202000031</t>
-  </si>
-  <si>
-    <t>7ff9010202000031</t>
-  </si>
-  <si>
     <t>000f161202000060</t>
   </si>
   <si>
     <t>7ff9010202000060</t>
   </si>
   <si>
-    <t>000f161202000032</t>
-  </si>
-  <si>
-    <t>7ff9010202000032</t>
-  </si>
-  <si>
-    <t>000f161202000036</t>
-  </si>
-  <si>
-    <t>7ff9010202000036</t>
-  </si>
-  <si>
-    <t>000f161202000037</t>
-  </si>
-  <si>
-    <t>7ff9010202000037</t>
-  </si>
-  <si>
     <t>000f161202000067</t>
   </si>
   <si>
     <t>7ff9010202000067</t>
   </si>
   <si>
-    <t>000f161202000081</t>
-  </si>
-  <si>
-    <t>7ff9010202000081</t>
-  </si>
-  <si>
     <t>000f161202000069</t>
   </si>
   <si>
     <t>7ff9010202000069</t>
   </si>
   <si>
-    <t>000f161202000082</t>
-  </si>
-  <si>
-    <t>7ff9010202000082</t>
-  </si>
-  <si>
     <t>000f161202000073</t>
   </si>
   <si>
@@ -686,12 +895,6 @@
     <t>7ff9010202000074</t>
   </si>
   <si>
-    <t>000f161202000084</t>
-  </si>
-  <si>
-    <t>7ff9010202000084</t>
-  </si>
-  <si>
     <t>000f161202000077</t>
   </si>
   <si>
@@ -722,12 +925,6 @@
     <t>7ff9010202000126</t>
   </si>
   <si>
-    <t>000f161202000088</t>
-  </si>
-  <si>
-    <t>7ff9010202000088</t>
-  </si>
-  <si>
     <t>000f161202000129</t>
   </si>
   <si>
@@ -740,24 +937,12 @@
     <t>7ff9010202000131</t>
   </si>
   <si>
-    <t>000f161202000092</t>
-  </si>
-  <si>
-    <t>7ff9010202000092</t>
-  </si>
-  <si>
     <t>000f161202000132</t>
   </si>
   <si>
     <t>7ff9010202000132</t>
   </si>
   <si>
-    <t>000f161202000095</t>
-  </si>
-  <si>
-    <t>7ff9010202000095</t>
-  </si>
-  <si>
     <t>000f161202000134</t>
   </si>
   <si>
@@ -770,66 +955,30 @@
     <t>7ff9010202000136</t>
   </si>
   <si>
-    <t>000f161202000098</t>
-  </si>
-  <si>
-    <t>7ff9010202000098</t>
-  </si>
-  <si>
-    <t>000f161202000100</t>
-  </si>
-  <si>
-    <t>7ff9010202000100</t>
-  </si>
-  <si>
     <t>000f161202000138</t>
   </si>
   <si>
     <t>7ff9010202000138</t>
   </si>
   <si>
-    <t>000f161202000102</t>
-  </si>
-  <si>
-    <t>7ff9010202000102</t>
-  </si>
-  <si>
     <t>000f161202000139</t>
   </si>
   <si>
     <t>7ff9010202000139</t>
   </si>
   <si>
-    <t>000f161202000103</t>
-  </si>
-  <si>
-    <t>7ff9010202000103</t>
-  </si>
-  <si>
     <t>000f161202000141</t>
   </si>
   <si>
     <t>7ff9010202000141</t>
   </si>
   <si>
-    <t>000f161202000104</t>
-  </si>
-  <si>
-    <t>7ff9010202000104</t>
-  </si>
-  <si>
     <t>000f161202000146</t>
   </si>
   <si>
     <t>7ff9010202000146</t>
   </si>
   <si>
-    <t>000f161202000106</t>
-  </si>
-  <si>
-    <t>7ff9010202000106</t>
-  </si>
-  <si>
     <t>000f161202000147</t>
   </si>
   <si>
@@ -842,92 +991,17 @@
     <t>7ff9010202000151</t>
   </si>
   <si>
-    <t>000f161202000108</t>
-  </si>
-  <si>
-    <t>7ff9010202000108</t>
-  </si>
-  <si>
     <t>000f161202000156</t>
   </si>
   <si>
     <t>7ff9010202000156</t>
-  </si>
-  <si>
-    <t>000f161202000112</t>
-  </si>
-  <si>
-    <t>7ff9010202000112</t>
-  </si>
-  <si>
-    <t>000f161202000113</t>
-  </si>
-  <si>
-    <t>7ff9010202000113</t>
-  </si>
-  <si>
-    <t>000f161202000116</t>
-  </si>
-  <si>
-    <t>7ff9010202000116</t>
-  </si>
-  <si>
-    <t>000f161202000118</t>
-  </si>
-  <si>
-    <t>7ff9010202000118</t>
-  </si>
-  <si>
-    <t>000f161202000153</t>
-  </si>
-  <si>
-    <t>7ff9010202000153</t>
-  </si>
-  <si>
-    <t>000f161202000161</t>
-  </si>
-  <si>
-    <t>7ff9010202000161</t>
-  </si>
-  <si>
-    <t>000f161202000162</t>
-  </si>
-  <si>
-    <t>7ff9010202000162</t>
-  </si>
-  <si>
-    <t>000f161202000163</t>
-  </si>
-  <si>
-    <t>7ff9010202000163</t>
-  </si>
-  <si>
-    <t>000f161202000164</t>
-  </si>
-  <si>
-    <t>7ff9010202000164</t>
-  </si>
-  <si>
-    <t>000f161202000166</t>
-  </si>
-  <si>
-    <t>7ff9010202000166</t>
-  </si>
-  <si>
-    <t>YL DEV EUI Power</t>
-  </si>
-  <si>
-    <t>YL EID Power</t>
-  </si>
-  <si>
-    <t>MC DEV EUI Power</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -965,8 +1039,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -981,6 +1063,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1025,7 +1113,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1039,10 +1127,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1349,10 +1443,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="23.28515625" customWidth="1"/>
+    <col min="11" max="11" width="255.7109375" style="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,195 +1552,195 @@
     <col min="3" max="3" width="36.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="33.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="12" width="9.140625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1576,12 +1766,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,194 +1786,194 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>276</v>
+        <v>60</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>168</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>182</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>188</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>288</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>282</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>196</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>198</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>202</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>174</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>278</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>290</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>210</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>248</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>286</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>292</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>206</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>242</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>232</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>258</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>262</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>214</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>220</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>238</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>254</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>280</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>266</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>204</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>284</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>192</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>250</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>272</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>294</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1792,7 +1982,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
@@ -1810,271 +2000,271 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>277</v>
+        <v>99</v>
       </c>
       <c r="B2">
         <v>8001</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>48</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>169</v>
+        <v>102</v>
       </c>
       <c r="B3">
         <v>8002</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>183</v>
+        <v>105</v>
       </c>
       <c r="B4">
         <v>8003</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>189</v>
+        <v>108</v>
       </c>
       <c r="B5">
         <v>8004</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>54</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>289</v>
+        <v>111</v>
       </c>
       <c r="B6">
         <v>8005</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>283</v>
+        <v>114</v>
       </c>
       <c r="B7">
         <v>8006</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>57</v>
+        <v>115</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>58</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>197</v>
+        <v>117</v>
       </c>
       <c r="B8">
         <v>8007</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>59</v>
+        <v>118</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>199</v>
+        <v>120</v>
       </c>
       <c r="B9">
         <v>8008</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>61</v>
+        <v>121</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>203</v>
+        <v>123</v>
       </c>
       <c r="B10">
         <v>8009</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>63</v>
+        <v>124</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>64</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>175</v>
+        <v>126</v>
       </c>
       <c r="B11">
         <v>8010</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>66</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>279</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>291</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>211</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>249</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>287</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>293</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>207</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>243</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>233</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>259</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>263</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>215</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>221</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>239</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>255</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>281</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>267</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>285</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>193</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>251</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>273</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>295</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2082,7 +2272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B64"/>
   <sheetViews>
@@ -2098,443 +2288,443 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>67</v>
+        <v>152</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>68</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>154</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>70</v>
+        <v>155</v>
       </c>
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>71</v>
+        <v>156</v>
       </c>
       <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>72</v>
+        <v>157</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>73</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>72</v>
+        <v>157</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>75</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>76</v>
+        <v>161</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>77</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>78</v>
+        <v>163</v>
       </c>
       <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>76</v>
+        <v>161</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>79</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>78</v>
+        <v>163</v>
       </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>80</v>
+        <v>165</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>77</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>81</v>
+        <v>166</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>80</v>
+        <v>165</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>79</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>80</v>
+        <v>165</v>
       </c>
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>82</v>
+        <v>167</v>
       </c>
       <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>83</v>
+        <v>168</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>84</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>83</v>
+        <v>168</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>86</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="B21" s="3"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>87</v>
+        <v>172</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>88</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>89</v>
+        <v>174</v>
       </c>
       <c r="B23" s="3"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>87</v>
+        <v>172</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>90</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>89</v>
+        <v>174</v>
       </c>
       <c r="B25" s="3"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>91</v>
+        <v>176</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>92</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>93</v>
+        <v>178</v>
       </c>
       <c r="B27" s="3"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>91</v>
+        <v>176</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>94</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>93</v>
+        <v>178</v>
       </c>
       <c r="B29" s="3"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>96</v>
+        <v>181</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>97</v>
+        <v>182</v>
       </c>
       <c r="B31" s="3"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>98</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>97</v>
+        <v>182</v>
       </c>
       <c r="B33" s="3"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>99</v>
+        <v>184</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>100</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>101</v>
+        <v>186</v>
       </c>
       <c r="B35" s="3"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>99</v>
+        <v>184</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>102</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>101</v>
+        <v>186</v>
       </c>
       <c r="B37" s="3"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>103</v>
+        <v>188</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>104</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>105</v>
+        <v>190</v>
       </c>
       <c r="B39" s="3"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>103</v>
+        <v>188</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>106</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>105</v>
+        <v>190</v>
       </c>
       <c r="B41" s="3"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>107</v>
+        <v>192</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>108</v>
+        <v>193</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>109</v>
+        <v>194</v>
       </c>
       <c r="B43" s="3"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>107</v>
+        <v>192</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>110</v>
+        <v>195</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>109</v>
+        <v>194</v>
       </c>
       <c r="B45" s="3"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>111</v>
+        <v>196</v>
       </c>
       <c r="B46" s="3"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>112</v>
+        <v>197</v>
       </c>
       <c r="B47" s="3"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>113</v>
+        <v>198</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>114</v>
+        <v>199</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>115</v>
+        <v>200</v>
       </c>
       <c r="B49" s="3"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>113</v>
+        <v>198</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>116</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>115</v>
+        <v>200</v>
       </c>
       <c r="B51" s="3"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>117</v>
+        <v>202</v>
       </c>
       <c r="B52" s="3"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>118</v>
+        <v>203</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>119</v>
+        <v>204</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>120</v>
+        <v>205</v>
       </c>
       <c r="B54" s="3"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>118</v>
+        <v>203</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>121</v>
+        <v>206</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>120</v>
+        <v>205</v>
       </c>
       <c r="B56" s="3"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>122</v>
+        <v>207</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>123</v>
+        <v>208</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>124</v>
+        <v>209</v>
       </c>
       <c r="B58" s="3"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>122</v>
+        <v>207</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>125</v>
+        <v>210</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>124</v>
+        <v>209</v>
       </c>
       <c r="B60" s="3"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>126</v>
+        <v>211</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>127</v>
+        <v>212</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>128</v>
+        <v>213</v>
       </c>
       <c r="B62" s="3"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>126</v>
+        <v>211</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>127</v>
+        <v>212</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>128</v>
+        <v>213</v>
       </c>
       <c r="B64" s="3"/>
     </row>
@@ -2543,7 +2733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2559,24 +2749,24 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>67</v>
+        <v>152</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>68</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>101</v>
+        <v>186</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>99</v>
+        <v>184</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>102</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2584,12 +2774,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2608,1141 +2798,1141 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>129</v>
+        <v>214</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>130</v>
+        <v>215</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>131</v>
+        <v>216</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>132</v>
+        <v>217</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>133</v>
+        <v>218</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>134</v>
+        <v>219</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>135</v>
+        <v>220</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>296</v>
+        <v>221</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>297</v>
+        <v>222</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>298</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>136</v>
+        <v>224</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>137</v>
+        <v>225</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>138</v>
+        <v>226</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>139</v>
+        <v>227</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>140</v>
+        <v>228</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>141</v>
+        <v>229</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>39</v>
+        <v>230</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>46</v>
+        <v>231</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>136</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>142</v>
+        <v>232</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>143</v>
+        <v>233</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>144</v>
+        <v>234</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>145</v>
+        <v>235</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>146</v>
+        <v>236</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>147</v>
+        <v>237</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>276</v>
+        <v>60</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>277</v>
+        <v>99</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>142</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>148</v>
+        <v>238</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>149</v>
+        <v>239</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>150</v>
+        <v>240</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>151</v>
+        <v>241</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>152</v>
+        <v>242</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>153</v>
+        <v>243</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>168</v>
+        <v>64</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>169</v>
+        <v>102</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>148</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>155</v>
+        <v>245</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>39</v>
+        <v>230</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>46</v>
+        <v>231</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>156</v>
+        <v>246</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>157</v>
+        <v>247</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>54</v>
+        <v>110</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>182</v>
+        <v>65</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>183</v>
+        <v>105</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>153</v>
+        <v>243</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>158</v>
+        <v>248</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>159</v>
+        <v>249</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>160</v>
+        <v>250</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>161</v>
+        <v>251</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>188</v>
+        <v>66</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>189</v>
+        <v>108</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>153</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>157</v>
+        <v>247</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>54</v>
+        <v>110</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>162</v>
+        <v>252</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>163</v>
+        <v>253</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>164</v>
+        <v>254</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>57</v>
+        <v>115</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>165</v>
+        <v>255</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>58</v>
+        <v>116</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>288</v>
+        <v>67</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>289</v>
+        <v>111</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>157</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>166</v>
+        <v>256</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>167</v>
+        <v>257</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>168</v>
+        <v>64</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>169</v>
+        <v>102</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>170</v>
+        <v>258</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>59</v>
+        <v>118</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>171</v>
+        <v>259</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>282</v>
+        <v>68</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>283</v>
+        <v>114</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>166</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>172</v>
+        <v>260</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>173</v>
+        <v>261</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>174</v>
+        <v>72</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>175</v>
+        <v>126</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>176</v>
+        <v>262</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>61</v>
+        <v>121</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>177</v>
+        <v>263</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>196</v>
+        <v>69</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>197</v>
+        <v>117</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>172</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>178</v>
+        <v>264</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>179</v>
+        <v>265</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>140</v>
+        <v>228</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>180</v>
+        <v>266</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>63</v>
+        <v>124</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>181</v>
+        <v>267</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>64</v>
+        <v>125</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>198</v>
+        <v>70</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>199</v>
+        <v>120</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>178</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>161</v>
+        <v>251</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>182</v>
+        <v>65</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>183</v>
+        <v>105</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>184</v>
+        <v>268</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>185</v>
+        <v>269</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>66</v>
+        <v>128</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>202</v>
+        <v>71</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>203</v>
+        <v>123</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>161</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>186</v>
+        <v>270</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>187</v>
+        <v>271</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>188</v>
+        <v>66</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>189</v>
+        <v>108</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>174</v>
+        <v>72</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>175</v>
+        <v>126</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>186</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>190</v>
+        <v>272</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>191</v>
+        <v>273</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>192</v>
+        <v>92</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>193</v>
+        <v>148</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>278</v>
+        <v>73</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>279</v>
+        <v>129</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>190</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>194</v>
+        <v>274</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>195</v>
+        <v>275</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>196</v>
+        <v>69</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>197</v>
+        <v>117</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>290</v>
+        <v>74</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>291</v>
+        <v>130</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>194</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>165</v>
+        <v>255</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>58</v>
+        <v>116</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>198</v>
+        <v>70</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>199</v>
+        <v>120</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>210</v>
+        <v>75</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>211</v>
+        <v>131</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>165</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>200</v>
+        <v>276</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>201</v>
+        <v>277</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>202</v>
+        <v>71</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>203</v>
+        <v>123</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>248</v>
+        <v>76</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>249</v>
+        <v>132</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>200</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>171</v>
+        <v>259</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>204</v>
+        <v>90</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>286</v>
+        <v>77</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>287</v>
+        <v>133</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>171</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>177</v>
+        <v>263</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>206</v>
+        <v>79</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>207</v>
+        <v>135</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>292</v>
+        <v>78</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>293</v>
+        <v>134</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>177</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>208</v>
+        <v>278</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>209</v>
+        <v>279</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>210</v>
+        <v>75</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>211</v>
+        <v>131</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>206</v>
+        <v>79</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>207</v>
+        <v>135</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>208</v>
+        <v>278</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>212</v>
+        <v>280</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>213</v>
+        <v>281</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>214</v>
+        <v>84</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>215</v>
+        <v>140</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>242</v>
+        <v>80</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>243</v>
+        <v>136</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>212</v>
+        <v>280</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>216</v>
+        <v>282</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>217</v>
+        <v>283</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>146</v>
+        <v>236</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>232</v>
+        <v>81</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>233</v>
+        <v>137</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>216</v>
+        <v>282</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>218</v>
+        <v>284</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>219</v>
+        <v>285</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>220</v>
+        <v>85</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>221</v>
+        <v>141</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>258</v>
+        <v>82</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>259</v>
+        <v>138</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>218</v>
+        <v>284</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>222</v>
+        <v>286</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>223</v>
+        <v>287</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>152</v>
+        <v>242</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>262</v>
+        <v>83</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>263</v>
+        <v>139</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>222</v>
+        <v>286</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>224</v>
+        <v>288</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>225</v>
+        <v>289</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>226</v>
+        <v>290</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>227</v>
+        <v>291</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>214</v>
+        <v>84</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>215</v>
+        <v>140</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>224</v>
+        <v>288</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>228</v>
+        <v>292</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>229</v>
+        <v>293</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>156</v>
+        <v>246</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>220</v>
+        <v>85</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>221</v>
+        <v>141</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>228</v>
+        <v>292</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>230</v>
+        <v>294</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>231</v>
+        <v>295</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>232</v>
+        <v>81</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>233</v>
+        <v>137</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>238</v>
+        <v>86</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>239</v>
+        <v>142</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>230</v>
+        <v>294</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>234</v>
+        <v>296</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>235</v>
+        <v>297</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>160</v>
+        <v>250</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>254</v>
+        <v>87</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>255</v>
+        <v>143</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>234</v>
+        <v>296</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>236</v>
+        <v>298</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>237</v>
+        <v>299</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>238</v>
+        <v>86</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>239</v>
+        <v>142</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>280</v>
+        <v>88</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>281</v>
+        <v>144</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>236</v>
+        <v>298</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>241</v>
+        <v>301</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>242</v>
+        <v>80</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>243</v>
+        <v>136</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>266</v>
+        <v>89</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>267</v>
+        <v>145</v>
       </c>
       <c r="K29" s="11" t="s">
-        <v>240</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>244</v>
+        <v>302</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>245</v>
+        <v>303</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>164</v>
+        <v>254</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>57</v>
+        <v>115</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>204</v>
+        <v>90</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
       <c r="K30" s="11" t="s">
-        <v>244</v>
+        <v>302</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>246</v>
+        <v>304</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>247</v>
+        <v>305</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>248</v>
+        <v>76</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>249</v>
+        <v>132</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>284</v>
+        <v>91</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>285</v>
+        <v>147</v>
       </c>
       <c r="K31" s="11" t="s">
-        <v>246</v>
+        <v>304</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>185</v>
+        <v>269</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>66</v>
+        <v>128</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>250</v>
+        <v>93</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>251</v>
+        <v>149</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>192</v>
+        <v>92</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>193</v>
+        <v>148</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>185</v>
+        <v>269</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>252</v>
+        <v>306</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>253</v>
+        <v>307</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>254</v>
+        <v>87</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>255</v>
+        <v>143</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>250</v>
+        <v>93</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>251</v>
+        <v>149</v>
       </c>
       <c r="K33" s="11" t="s">
-        <v>252</v>
+        <v>306</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>256</v>
+        <v>308</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>257</v>
+        <v>309</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>258</v>
+        <v>82</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>259</v>
+        <v>138</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>272</v>
+        <v>94</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>273</v>
+        <v>150</v>
       </c>
       <c r="K34" s="11" t="s">
-        <v>256</v>
+        <v>308</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>260</v>
+        <v>310</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>261</v>
+        <v>311</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>262</v>
+        <v>83</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>263</v>
+        <v>139</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>294</v>
+        <v>95</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>295</v>
+        <v>151</v>
       </c>
       <c r="K35" s="11" t="s">
-        <v>260</v>
+        <v>310</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>264</v>
+        <v>312</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>265</v>
+        <v>313</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>266</v>
+        <v>89</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>267</v>
+        <v>145</v>
       </c>
       <c r="K36" s="11" t="s">
-        <v>264</v>
+        <v>312</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>268</v>
+        <v>314</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>269</v>
+        <v>315</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>170</v>
+        <v>258</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>59</v>
+        <v>118</v>
       </c>
       <c r="K37" s="11" t="s">
-        <v>268</v>
+        <v>314</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>270</v>
+        <v>316</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>271</v>
+        <v>317</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>272</v>
+        <v>94</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>273</v>
+        <v>150</v>
       </c>
       <c r="K38" s="11" t="s">
-        <v>270</v>
+        <v>316</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>274</v>
+        <v>318</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>275</v>
+        <v>319</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>276</v>
+        <v>60</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>277</v>
+        <v>99</v>
       </c>
       <c r="K39" s="11" t="s">
-        <v>274</v>
+        <v>318</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>252</v>
+        <v>306</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>253</v>
+        <v>307</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>278</v>
+        <v>73</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>279</v>
+        <v>129</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>252</v>
+        <v>306</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>230</v>
+        <v>294</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>231</v>
+        <v>295</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>280</v>
+        <v>88</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>281</v>
+        <v>144</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>230</v>
+        <v>294</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
-        <v>176</v>
+        <v>262</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>61</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3" t="s">
-        <v>282</v>
+        <v>68</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>283</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3" t="s">
-        <v>284</v>
+        <v>91</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>285</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3" t="s">
-        <v>286</v>
+        <v>77</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>287</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
-        <v>288</v>
+        <v>67</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>289</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3" t="s">
-        <v>290</v>
+        <v>74</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>291</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
-        <v>292</v>
+        <v>78</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>293</v>
+        <v>134</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3" t="s">
-        <v>180</v>
+        <v>266</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>63</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3" t="s">
-        <v>294</v>
+        <v>95</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>295</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3" t="s">
-        <v>184</v>
+        <v>268</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update lib regarding to the change of formula
</commit_message>
<xml_diff>
--- a/Resources/testdata/TestData.xlsx
+++ b/Resources/testdata/TestData.xlsx
@@ -20,7 +20,7 @@
     <sheet name="yl_command_test" sheetId="6" r:id="rId6"/>
     <sheet name="device info" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -56,11 +56,11 @@
   </si>
   <si>
     <t>Scheduled msg 
-not Reived</t>
+not Received</t>
   </si>
   <si>
     <t>Scheduled msg 
-Reived</t>
+Received</t>
   </si>
   <si>
     <t>Scheduled msg 
@@ -73,31 +73,31 @@
     <t>17-09-24 ~ 17-09-25</t>
   </si>
   <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>96.30%</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>66.67%</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>0.00%</t>
+  </si>
+  <si>
     <t>['7ff9010202000024', '7ff9010202000026', '7ff9010202000031', '7ff9010202000032', '7ff9010202000037', '7ff9010202000084', '7ff9010202000092', '7ff9010202000095', '7ff9010202000098', '7ff9010202000108', '7ff9010202000116', '7ff9010202000153', '7ff9010202000162', '7ff9010202000163', '7ff9010202000164', '7ff9010202000166']</t>
-  </si>
-  <si>
-    <t>54</t>
-  </si>
-  <si>
-    <t>52</t>
-  </si>
-  <si>
-    <t>96.30%</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>66.67%</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>0.00%</t>
   </si>
   <si>
     <t>Info</t>
@@ -1446,12 +1446,12 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
@@ -1501,34 +1501,34 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1552,8 +1552,8 @@
     <col min="3" max="3" width="36.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="33.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.140625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="15" width="9.140625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add time out commands response.
</commit_message>
<xml_diff>
--- a/Resources/testdata/TestData.xlsx
+++ b/Resources/testdata/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="320">
   <si>
     <t>Date
 Period</t>
@@ -226,9 +226,6 @@
     <t>2b7e151628aed2a6abf7158809cf4f3c</t>
   </si>
   <si>
-    <t>YL POW</t>
-  </si>
-  <si>
     <t>000f161202000022</t>
   </si>
   <si>
@@ -995,6 +992,9 @@
   </si>
   <si>
     <t>7ff9010202000156</t>
+  </si>
+  <si>
+    <t>MC POW</t>
   </si>
 </sst>
 </file>
@@ -1445,7 +1445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1542,7 +1542,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,7 +1629,7 @@
         <v>36</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>37</v>
@@ -1768,10 +1768,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1784,7 +1784,7 @@
     <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>55</v>
       </c>
@@ -1801,9 +1801,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>60</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>223</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>61</v>
@@ -1812,168 +1812,313 @@
         <v>62</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="11" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="11" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="11" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="11" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="11" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="11" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="11" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="11" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="11" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="11" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="11" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="11" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="11" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="11" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="11" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="11" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="11" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="11" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="11" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="11" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="11" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="11" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="11" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="12" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="41" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F41" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="42" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    <row r="43" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F43" s="11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="44" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F44" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F45" s="11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="46" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F46" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="47" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F47" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="48" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F48" s="11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F50" s="11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F51" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F52" s="11" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F53" s="11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="55" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F55" s="11" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F56" s="11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F57" s="11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F58" s="11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F59" s="11" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="60" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F60" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="61" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F61" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="62" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F62" s="11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="63" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F63" s="11" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1984,10 +2129,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2000,272 +2145,412 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>63</v>
+        <v>319</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
         <v>96</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>97</v>
-      </c>
-      <c r="E1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B2">
         <v>8001</v>
       </c>
+      <c r="C2" s="11" t="s">
+        <v>224</v>
+      </c>
       <c r="D2" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>102</v>
+      <c r="A3" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="B3">
         <v>8002</v>
       </c>
+      <c r="C3" s="11" t="s">
+        <v>232</v>
+      </c>
       <c r="D3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>104</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>105</v>
+      <c r="A4" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="B4">
         <v>8003</v>
       </c>
+      <c r="C4" s="11" t="s">
+        <v>238</v>
+      </c>
       <c r="D4" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>108</v>
+      <c r="A5" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="B5">
         <v>8004</v>
       </c>
+      <c r="C5" s="11" t="s">
+        <v>244</v>
+      </c>
       <c r="D5" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B6">
-        <v>8005</v>
+        <v>8007</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>256</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B7">
-        <v>8006</v>
+        <v>8008</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>260</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B8">
-        <v>8007</v>
+        <v>8009</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>264</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B9">
-        <v>8008</v>
-      </c>
-      <c r="D9" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>122</v>
+      <c r="C9" s="11" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B10">
-        <v>8009</v>
-      </c>
-      <c r="D10" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>125</v>
+      <c r="C10" s="11" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B11">
-        <v>8010</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="A11" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>128</v>
+      <c r="C11" s="11" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>129</v>
+      <c r="A12" s="6"/>
+      <c r="C12" s="11" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>130</v>
+      <c r="A13" s="3"/>
+      <c r="C13" s="11" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>131</v>
+      <c r="A14" s="3"/>
+      <c r="C14" s="11" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>132</v>
+      <c r="A15" s="3"/>
+      <c r="C15" s="11" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>149</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="C16" s="11" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="C17" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="C18" s="11" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="C19" s="11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="C20" s="11" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="C21" s="11" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="C22" s="11" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="C23" s="11" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="C24" s="11" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="C25" s="11" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="C26" s="11" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="C27" s="11" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="C28" s="11" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="C29" s="11" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="C30" s="11" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="C31" s="11" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>150</v>
-      </c>
+      <c r="A33" s="3"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>151</v>
-      </c>
+      <c r="A34" s="3"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="11"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="11"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="11"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="11"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="11"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="11"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="11"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="11"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="11"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="11"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="11"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="11"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="11"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="11"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="11"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="11"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="11"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="11"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="11"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="11"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="11"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="11"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="11"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2276,8 +2561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2288,443 +2573,443 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B21" s="3"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B23" s="3"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B25" s="3"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B27" s="3"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B29" s="3"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B31" s="3"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B33" s="3"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B35" s="3"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B37" s="3"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>188</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B39" s="3"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B41" s="3"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B43" s="3"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B45" s="3"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B46" s="3"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B47" s="3"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B49" s="3"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B51" s="3"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B52" s="3"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B54" s="3"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B56" s="3"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B58" s="3"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B60" s="3"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B62" s="3"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B64" s="3"/>
     </row>
@@ -2749,24 +3034,24 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2776,10 +3061,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="H2" sqref="H2:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2793,1146 +3078,1269 @@
     <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="H2" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="K2" s="11" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>60</v>
       </c>
       <c r="J3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="K3" s="11" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="E10" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="L19" s="11" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="K21" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="L21" s="11" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="D23" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="L24" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="D25" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="K26" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="L26" s="11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="D27" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="L27" s="11" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="L28" s="11" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="L29" s="11" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="D30" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="L30" s="11" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="L31" s="11" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="K33" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="L33" s="11" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>307</v>
+      </c>
+      <c r="L34" s="11" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K35" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="L35" s="11" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="K36" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="L36" s="11" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="J9" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="K9" s="11" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="K19" s="11" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="K20" s="11" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="K21" s="11" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="K22" s="11" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I23" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="I24" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="K24" s="11" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="K25" s="11" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="I26" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="K26" s="11" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="I27" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="K27" s="11" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="I28" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="K28" s="11" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="I29" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="K29" s="11" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="I30" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="K30" s="11" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="I31" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="J31" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="K31" s="11" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="K37" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="L37" s="11" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="I32" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="K32" s="3" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="K33" s="11" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I34" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="K34" s="11" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="K35" s="11" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="K36" s="11" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="B37" s="3" t="s">
+      <c r="K38" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="K37" s="11" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="L38" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="B38" s="3" t="s">
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="K38" s="11" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>318</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>319</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>60</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K39" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="L39" s="11" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>307</v>
-      </c>
       <c r="C40" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K40" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="L40" s="3" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>295</v>
-      </c>
       <c r="C41" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K41" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="L41" s="3" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FW 1.0.12-STB and LUA 2.2.81-STG integration
</commit_message>
<xml_diff>
--- a/Resources/testdata/TestData.xlsx
+++ b/Resources/testdata/TestData.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="report" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="enviornment" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="appserver" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="devices" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="yl_command" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="yl_command_test" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="device info" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="report" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="enviornment" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="appserver" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="devices" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="yl_command" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="yl_command_test" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="device info" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="326">
   <si>
     <t>Date
 Period</t>
@@ -183,7 +183,7 @@
     <t>2bc5f7428c45996d586710a6a8538da3</t>
   </si>
   <si>
-    <t>c1de11d2bbe3a01b1a5b83304af392e4</t>
+    <t>f46e90ea5336797169119a3f64d86afb</t>
   </si>
   <si>
     <t>f1c512887264a3a3c486cd8a15ab9310</t>
@@ -192,7 +192,7 @@
     <t>3eaa2cbe9a15ce0119f26a518a234c9d</t>
   </si>
   <si>
-    <t>4aae97a44e57eeee6d31e34b5a9a0cef</t>
+    <t>e2cdac8a1cbcb24f7849c8d77748abe1</t>
   </si>
   <si>
     <t>APP_UPDATE</t>
@@ -1016,51 +1016,51 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="@" numFmtId="165"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="6">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF66FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FFFF66FF"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -1079,21 +1079,21 @@
     </fill>
   </fills>
   <borders count="3">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
       <top/>
@@ -1101,376 +1101,185 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="5" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="5" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="3" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" name="Comma" xfId="1"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
-    <cellStyle builtinId="4" name="Currency" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="5" name="Percent" xfId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFFFCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF66FF"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF00B050"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100">
-      <selection activeCell="D9" activeCellId="0" pane="topLeft" sqref="D9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="21.0040485829959"/>
-    <col customWidth="1" max="3" min="2" style="1" width="7.85425101214575"/>
-    <col customWidth="1" max="4" min="4" style="1" width="17.7085020242915"/>
-    <col customWidth="1" max="5" min="5" style="1" width="17.4251012145749"/>
-    <col customWidth="1" max="6" min="6" style="1" width="15.7125506072875"/>
-    <col customWidth="1" max="7" min="7" style="1" width="24.1457489878543"/>
-    <col customWidth="1" max="10" min="8" style="1" width="23.2793522267206"/>
-    <col customWidth="1" max="11" min="11" style="2" width="255.712550607287"/>
-    <col customWidth="1" max="1025" min="12" style="1" width="8.570850202429151"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.0040485829959"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="7.85425101214575"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.7125506072875"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.1457489878543"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="1" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="255.712550607287"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="45" r="1" s="13" spans="1:11">
+    <row r="1" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1505,7 +1314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="2" s="13" spans="1:11">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1541,36 +1350,39 @@
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F16" activeCellId="0" pane="topLeft" sqref="F16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="21.4251012145749"/>
-    <col customWidth="1" max="2" min="2" style="1" width="36.5708502024291"/>
-    <col customWidth="1" max="3" min="3" style="1" width="36.8542510121458"/>
-    <col customWidth="1" max="4" min="4" style="1" width="33.1417004048583"/>
-    <col customWidth="1" max="5" min="5" style="1" width="34.2834008097166"/>
-    <col customWidth="1" max="6" min="6" style="1" width="34.5708502024291"/>
-    <col customWidth="1" max="1025" min="7" style="1" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="36.5708502024291"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.8542510121458"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="33.1417004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="34.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="34.5708502024291"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.1417004048583"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="13" spans="1:6">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -1590,7 +1402,7 @@
         <v>26</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="2" s="13" spans="1:6">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -1610,7 +1422,7 @@
         <v>31</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.85" r="3" s="13" spans="1:6">
+    <row r="3" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
@@ -1630,7 +1442,7 @@
         <v>36</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="4" s="13" spans="1:6">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>37</v>
       </c>
@@ -1650,7 +1462,7 @@
         <v>38</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="5" s="13" spans="1:6">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>39</v>
       </c>
@@ -1670,7 +1482,7 @@
         <v>42</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="6" s="13" spans="1:6">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>43</v>
       </c>
@@ -1690,7 +1502,7 @@
         <v>44</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="7" s="13" spans="1:6">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>45</v>
       </c>
@@ -1710,7 +1522,7 @@
         <v>46</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="8" s="13" spans="1:6">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>47</v>
       </c>
@@ -1730,7 +1542,7 @@
         <v>46</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="9" s="13" spans="1:6">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>48</v>
       </c>
@@ -1746,11 +1558,11 @@
       <c r="E9" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="10" s="13" spans="1:6">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>54</v>
       </c>
@@ -1770,7 +1582,7 @@
         <v>55</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="11" s="13" spans="1:6">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>56</v>
       </c>
@@ -1790,56 +1602,59 @@
         <v>58</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="12" s="13" spans="1:6">
-      <c r="A12" s="4" t="n"/>
-      <c r="B12" s="4" t="n"/>
-      <c r="C12" s="4" t="n"/>
-      <c r="D12" s="4" t="n"/>
-      <c r="E12" s="4" t="n"/>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" display="http://10.10.20.152:83" ref="B2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" display="http://10.10.10.125:83" ref="C2" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" display="http://10.10.20.208:83" ref="D2" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" display="http://10.10.10.125:83" ref="E2" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" display="https://10.10.20.152:8080" ref="B11" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" display="https://10.10.20.125:8080" ref="C11" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" display="https://10.10.20.208:8080" ref="D11" r:id="rId7"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" display="https://10.10.10.125:8080" ref="E11" r:id="rId8"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" display="https://10.10.20.125:8080" ref="F11" r:id="rId9"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://10.10.20.152:83"/>
+    <hyperlink ref="C2" r:id="rId2" display="http://10.10.10.125:83"/>
+    <hyperlink ref="D2" r:id="rId3" display="http://10.10.20.208:83"/>
+    <hyperlink ref="E2" r:id="rId4" display="http://10.10.10.125:83"/>
+    <hyperlink ref="B11" r:id="rId5" display="https://10.10.20.152:8080"/>
+    <hyperlink ref="C11" r:id="rId6" display="https://10.10.20.125:8080"/>
+    <hyperlink ref="D11" r:id="rId7" display="https://10.10.20.208:8080"/>
+    <hyperlink ref="E11" r:id="rId8" display="https://10.10.10.125:8080"/>
+    <hyperlink ref="F11" r:id="rId9" display="https://10.10.20.125:8080"/>
   </hyperlinks>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D8" activeCellId="0" pane="topLeft" sqref="D8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="16.8542510121458"/>
-    <col customWidth="1" max="2" min="2" style="1" width="17.2834008097166"/>
-    <col customWidth="1" max="3" min="3" style="1" width="33.2834008097166"/>
-    <col customWidth="1" max="4" min="4" style="1" width="16.1376518218624"/>
-    <col customWidth="1" max="5" min="5" style="1" width="23.5748987854251"/>
-    <col customWidth="1" max="6" min="6" style="1" width="8.570850202429151"/>
-    <col customWidth="1" max="7" min="7" style="1" width="16.8542510121458"/>
-    <col customWidth="1" max="1025" min="8" style="1" width="8.570850202429151"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="33.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.1376518218624"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.5748987854251"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.8542510121458"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="13" spans="1:6">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
@@ -1855,10 +1670,10 @@
       <c r="E1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="1" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="2" s="13" spans="1:6">
-      <c r="A2" s="6" t="s">
+      <c r="F1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>66</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1870,349 +1685,352 @@
       <c r="D2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="1" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="3" s="13" spans="1:6">
-      <c r="F3" s="6" t="s">
+      <c r="F2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F3" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="4" s="13" spans="1:6">
-      <c r="F4" s="6" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F4" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="5" s="13" spans="1:6">
-      <c r="F5" s="6" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F5" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="6" s="13" spans="1:6">
-      <c r="F6" s="6" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F6" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="7" s="13" spans="1:6">
-      <c r="F7" s="6" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F7" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="8" s="13" spans="1:6">
-      <c r="F8" s="6" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F8" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="9" s="13" spans="1:6">
-      <c r="F9" s="6" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F9" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="10" s="13" spans="1:6">
-      <c r="F10" s="6" t="s">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F10" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="11" s="13" spans="1:6">
-      <c r="F11" s="6" t="s">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F11" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="12" s="13" spans="1:6">
-      <c r="F12" s="6" t="s">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F12" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="13" s="13" spans="1:6">
-      <c r="F13" s="6" t="s">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F13" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="14" s="13" spans="1:6">
-      <c r="F14" s="6" t="s">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F14" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="15" s="13" spans="1:6">
-      <c r="F15" s="6" t="s">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F15" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="16" s="13" spans="1:6">
-      <c r="F16" s="6" t="s">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F16" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="17" s="13" spans="1:6">
-      <c r="F17" s="6" t="s">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F17" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="18" s="13" spans="1:6">
-      <c r="F18" s="6" t="s">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F18" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="19" s="13" spans="1:6">
-      <c r="F19" s="6" t="s">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F19" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="20" s="13" spans="1:6">
-      <c r="F20" s="6" t="s">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F20" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="21" s="13" spans="1:6">
-      <c r="F21" s="6" t="s">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F21" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="22" s="13" spans="1:6">
-      <c r="F22" s="6" t="s">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F22" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="23" s="13" spans="1:6">
-      <c r="F23" s="6" t="s">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F23" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="24" s="13" spans="1:6">
-      <c r="F24" s="6" t="s">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F24" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="25" s="13" spans="1:6">
-      <c r="F25" s="6" t="s">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F25" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="26" s="13" spans="1:6">
-      <c r="F26" s="6" t="s">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F26" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="27" s="13" spans="1:6">
-      <c r="F27" s="6" t="s">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F27" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="28" s="13" spans="1:6">
-      <c r="F28" s="6" t="s">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F28" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="29" s="13" spans="1:6">
-      <c r="F29" s="6" t="s">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F29" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="30" s="13" spans="1:6">
-      <c r="F30" s="6" t="s">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F30" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="31" s="13" spans="1:6">
-      <c r="F31" s="6" t="s">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F31" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="32" s="13" spans="1:6">
-      <c r="F32" s="7" t="s">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F32" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="33" s="13" spans="1:6">
-      <c r="F33" s="6" t="s">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F33" s="7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="34" s="13" spans="1:6">
-      <c r="F34" s="7" t="s">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F34" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="35" s="13" spans="1:6">
-      <c r="F35" s="7" t="s">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F35" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="36" s="13" spans="1:6">
-      <c r="F36" s="7" t="s">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F36" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="37" s="13" spans="1:6">
-      <c r="F37" s="6" t="s">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F37" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="38" s="13" spans="1:6">
-      <c r="F38" s="6" t="s">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F38" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="39" s="13" spans="1:6">
-      <c r="F39" s="6" t="s">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F39" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="40" s="13" spans="1:6">
-      <c r="F40" s="6" t="s">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F40" s="7" t="s">
         <v>107</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="41" s="13" spans="1:6">
-      <c r="F41" s="6" t="s">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F41" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="42" s="13" spans="1:6">
-      <c r="F42" s="7" t="s">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F42" s="8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="43" s="13" spans="1:6">
-      <c r="F43" s="6" t="s">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F43" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="44" s="13" spans="1:6">
-      <c r="F44" s="6" t="s">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F44" s="7" t="s">
         <v>111</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="45" s="13" spans="1:6">
-      <c r="F45" s="6" t="s">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F45" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="46" s="13" spans="1:6">
-      <c r="F46" s="6" t="s">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F46" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="47" s="13" spans="1:6">
-      <c r="F47" s="6" t="s">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F47" s="7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="48" s="13" spans="1:6">
-      <c r="F48" s="6" t="s">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F48" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="49" s="13" spans="1:6">
-      <c r="F49" s="6" t="s">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F49" s="7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="50" s="13" spans="1:6">
-      <c r="F50" s="6" t="s">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F50" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="51" s="13" spans="1:6">
-      <c r="F51" s="6" t="s">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F51" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="52" s="13" spans="1:6">
-      <c r="F52" s="6" t="s">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F52" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="53" s="13" spans="1:6">
-      <c r="F53" s="6" t="s">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F53" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="54" s="13" spans="1:6">
-      <c r="F54" s="6" t="s">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F54" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="55" s="13" spans="1:6">
-      <c r="F55" s="6" t="s">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F55" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="56" s="13" spans="1:6">
-      <c r="F56" s="6" t="s">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F56" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="57" s="13" spans="1:6">
-      <c r="F57" s="6" t="s">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F57" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="58" s="13" spans="1:6">
-      <c r="F58" s="6" t="s">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F58" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="59" s="13" spans="1:6">
-      <c r="F59" s="6" t="s">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F59" s="7" t="s">
         <v>126</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="60" s="13" spans="1:6">
-      <c r="F60" s="6" t="s">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F60" s="7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="61" s="13" spans="1:6">
-      <c r="F61" s="6" t="s">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F61" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="62" s="13" spans="1:6">
-      <c r="F62" s="6" t="s">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F62" s="7" t="s">
         <v>129</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="63" s="13" spans="1:6">
-      <c r="F63" s="6" t="s">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F63" s="7" t="s">
         <v>130</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="16.5668016194332"/>
-    <col customWidth="1" max="2" min="2" style="1" width="11.5708502024291"/>
-    <col customWidth="1" max="3" min="3" style="1" width="19.7085020242915"/>
-    <col customWidth="1" max="5" min="4" style="1" width="16.5668016194332"/>
-    <col customWidth="1" max="1025" min="6" style="1" width="8.570850202429151"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.5708502024291"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="16.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="13" spans="1:5">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C1" s="1" t="n"/>
+      <c r="C1" s="0"/>
       <c r="D1" s="1" t="s">
         <v>132</v>
       </c>
@@ -2220,428 +2038,431 @@
         <v>133</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="2" s="13" spans="1:5">
-      <c r="A2" s="8" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
         <v>134</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>8001</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>135</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>134</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="3" s="13" spans="1:5">
-      <c r="A3" s="8" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
         <v>137</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>8002</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>137</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="4" s="13" spans="1:5">
-      <c r="A4" s="8" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
         <v>140</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>8003</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="9" t="s">
         <v>140</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="5" s="13" spans="1:5">
-      <c r="A5" s="8" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
         <v>143</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>8004</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="6" s="13" spans="1:5">
-      <c r="A6" s="8" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
         <v>146</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>8007</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="9" t="s">
         <v>149</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="7" s="13" spans="1:5">
-      <c r="A7" s="8" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
         <v>150</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>8008</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="9" t="s">
         <v>153</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="8" s="13" spans="1:5">
-      <c r="A8" s="8" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
         <v>149</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>8009</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="9" t="s">
         <v>156</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="9" s="13" spans="1:5">
-      <c r="A9" s="8" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>157</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="10" s="13" spans="1:5">
-      <c r="A10" s="8" t="s">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="11" s="13" spans="1:5">
-      <c r="A11" s="8" t="s">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="12" s="13" spans="1:5">
-      <c r="A12" s="4" t="n"/>
-      <c r="C12" s="6" t="s">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4"/>
+      <c r="C12" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="13" s="13" spans="1:5">
-      <c r="A13" s="8" t="n"/>
-      <c r="C13" s="6" t="s">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9"/>
+      <c r="C13" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="14" s="13" spans="1:5">
-      <c r="A14" s="8" t="n"/>
-      <c r="C14" s="6" t="s">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9"/>
+      <c r="C14" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="15" s="13" spans="1:5">
-      <c r="A15" s="8" t="n"/>
-      <c r="C15" s="6" t="s">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9"/>
+      <c r="C15" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="16" s="13" spans="1:5">
-      <c r="A16" s="8" t="n"/>
-      <c r="C16" s="6" t="s">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9"/>
+      <c r="C16" s="7" t="s">
         <v>165</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="17" s="13" spans="1:5">
-      <c r="A17" s="8" t="n"/>
-      <c r="C17" s="6" t="s">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9"/>
+      <c r="C17" s="7" t="s">
         <v>166</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="18" s="13" spans="1:5">
-      <c r="A18" s="8" t="n"/>
-      <c r="C18" s="6" t="s">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9"/>
+      <c r="C18" s="7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="19" s="13" spans="1:5">
-      <c r="A19" s="8" t="n"/>
-      <c r="C19" s="6" t="s">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9"/>
+      <c r="C19" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="20" s="13" spans="1:5">
-      <c r="A20" s="8" t="n"/>
-      <c r="C20" s="6" t="s">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9"/>
+      <c r="C20" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="21" s="13" spans="1:5">
-      <c r="A21" s="8" t="n"/>
-      <c r="C21" s="6" t="s">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="9"/>
+      <c r="C21" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="22" s="13" spans="1:5">
-      <c r="A22" s="8" t="n"/>
-      <c r="C22" s="6" t="s">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9"/>
+      <c r="C22" s="7" t="s">
         <v>171</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="23" s="13" spans="1:5">
-      <c r="A23" s="8" t="n"/>
-      <c r="C23" s="6" t="s">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9"/>
+      <c r="C23" s="7" t="s">
         <v>172</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="24" s="13" spans="1:5">
-      <c r="A24" s="8" t="n"/>
-      <c r="C24" s="6" t="s">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9"/>
+      <c r="C24" s="7" t="s">
         <v>173</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="25" s="13" spans="1:5">
-      <c r="A25" s="8" t="n"/>
-      <c r="C25" s="6" t="s">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9"/>
+      <c r="C25" s="7" t="s">
         <v>174</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="26" s="13" spans="1:5">
-      <c r="A26" s="8" t="n"/>
-      <c r="C26" s="6" t="s">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="9"/>
+      <c r="C26" s="7" t="s">
         <v>175</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="27" s="13" spans="1:5">
-      <c r="A27" s="8" t="n"/>
-      <c r="C27" s="6" t="s">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="9"/>
+      <c r="C27" s="7" t="s">
         <v>176</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="28" s="13" spans="1:5">
-      <c r="A28" s="8" t="n"/>
-      <c r="C28" s="6" t="s">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="9"/>
+      <c r="C28" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="29" s="13" spans="1:5">
-      <c r="A29" s="8" t="n"/>
-      <c r="C29" s="6" t="s">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="9"/>
+      <c r="C29" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="30" s="13" spans="1:5">
-      <c r="A30" s="8" t="n"/>
-      <c r="C30" s="6" t="s">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="9"/>
+      <c r="C30" s="7" t="s">
         <v>179</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="31" s="13" spans="1:5">
-      <c r="A31" s="8" t="n"/>
-      <c r="C31" s="6" t="s">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9"/>
+      <c r="C31" s="7" t="s">
         <v>180</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="32" s="13" spans="1:5">
-      <c r="A32" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="33" s="13" spans="1:5">
-      <c r="A33" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="34" s="13" spans="1:5">
-      <c r="A34" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="35" s="13" spans="1:5">
-      <c r="A35" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="36" s="13" spans="1:5">
-      <c r="A36" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="37" s="13" spans="1:5">
-      <c r="A37" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="38" s="13" spans="1:5">
-      <c r="A38" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="39" s="13" spans="1:5">
-      <c r="A39" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="40" s="13" spans="1:5">
-      <c r="A40" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="41" s="13" spans="1:5">
-      <c r="A41" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="42" s="13" spans="1:5">
-      <c r="A42" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="43" s="13" spans="1:5">
-      <c r="A43" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="44" s="13" spans="1:5">
-      <c r="A44" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="45" s="13" spans="1:5">
-      <c r="A45" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="46" s="13" spans="1:5">
-      <c r="A46" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="47" s="13" spans="1:5">
-      <c r="A47" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="48" s="13" spans="1:5">
-      <c r="A48" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="49" s="13" spans="1:5">
-      <c r="A49" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="50" s="13" spans="1:5">
-      <c r="A50" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="51" s="13" spans="1:5">
-      <c r="A51" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="52" s="13" spans="1:5">
-      <c r="A52" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="53" s="13" spans="1:5">
-      <c r="A53" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="54" s="13" spans="1:5">
-      <c r="A54" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="55" s="13" spans="1:5">
-      <c r="A55" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="56" s="13" spans="1:5">
-      <c r="A56" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="57" s="13" spans="1:5">
-      <c r="A57" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="58" s="13" spans="1:5">
-      <c r="A58" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="59" s="13" spans="1:5">
-      <c r="A59" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="60" s="13" spans="1:5">
-      <c r="A60" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="61" s="13" spans="1:5">
-      <c r="A61" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="62" s="13" spans="1:5">
-      <c r="A62" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="63" s="13" spans="1:5">
-      <c r="A63" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="64" s="13" spans="1:5">
-      <c r="A64" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="65" s="13" spans="1:5">
-      <c r="A65" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="66" s="13" spans="1:5">
-      <c r="A66" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="67" s="13" spans="1:5">
-      <c r="A67" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="68" s="13" spans="1:5">
-      <c r="A68" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="69" s="13" spans="1:5">
-      <c r="A69" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="70" s="13" spans="1:5">
-      <c r="A70" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="71" s="13" spans="1:5">
-      <c r="A71" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="72" s="13" spans="1:5">
-      <c r="A72" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="73" s="13" spans="1:5">
-      <c r="A73" s="6" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="74" s="13" spans="1:5">
-      <c r="A74" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="75" s="13" spans="1:5">
-      <c r="A75" s="8" t="n"/>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="9"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="9"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="9"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="7"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="7"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="7"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="9"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="9"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="7"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="7"/>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="7"/>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="9"/>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="7"/>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="7"/>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="7"/>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="9"/>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="7"/>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="9"/>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="9"/>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="7"/>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="7"/>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="7"/>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="7"/>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="9"/>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="7"/>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="7"/>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="7"/>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="7"/>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="7"/>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="7"/>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="7"/>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="7"/>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="9"/>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="7"/>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="7"/>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="7"/>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="7"/>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="7"/>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="7"/>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="7"/>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="9"/>
+    </row>
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="9"/>
     </row>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="35"/>
-    <col customWidth="1" max="2" min="2" style="1" width="53.2793522267207"/>
-    <col customWidth="1" max="1025" min="3" style="1" width="8.570850202429151"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="53.2793522267207"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="13" spans="1:2">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>181</v>
       </c>
@@ -2649,467 +2470,470 @@
         <v>182</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="2" s="13" spans="1:2">
-      <c r="A2" s="8" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="3" s="13" spans="1:2">
-      <c r="A3" s="8" t="s">
+      <c r="B2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="B3" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="4" s="13" spans="1:2">
-      <c r="A4" s="8" t="s">
+      <c r="B3" s="9"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="B4" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="5" s="13" spans="1:2">
-      <c r="A5" s="8" t="s">
+      <c r="B4" s="9"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>187</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="6" s="13" spans="1:2">
-      <c r="A6" s="8" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="B6" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="7" s="13" spans="1:2">
-      <c r="A7" s="8" t="s">
+      <c r="B6" s="9"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>189</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="8" s="13" spans="1:2">
-      <c r="A8" s="8" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="B8" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="9" s="13" spans="1:2">
-      <c r="A9" s="9" t="s">
+      <c r="B8" s="9"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>191</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="10" s="13" spans="1:2">
-      <c r="A10" s="8" t="s">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="B10" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="11" s="13" spans="1:2">
-      <c r="A11" s="9" t="s">
+      <c r="B10" s="9"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>193</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="12" s="13" spans="1:2">
-      <c r="A12" s="8" t="s">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="B12" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="13" s="13" spans="1:2">
-      <c r="A13" s="8" t="s">
+      <c r="B12" s="9"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="9" t="s">
         <v>191</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="14" s="13" spans="1:2">
-      <c r="A14" s="9" t="s">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="B14" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="15" s="13" spans="1:2">
-      <c r="A15" s="8" t="s">
+      <c r="B14" s="9"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>193</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="16" s="13" spans="1:2">
-      <c r="A16" s="8" t="s">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="B16" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="17" s="13" spans="1:2">
-      <c r="A17" s="8" t="s">
+      <c r="B16" s="9"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="B17" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="18" s="13" spans="1:2">
-      <c r="A18" s="8" t="s">
+      <c r="B17" s="9"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>198</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="19" s="13" spans="1:2">
-      <c r="A19" s="8" t="s">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="B19" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="20" s="13" spans="1:2">
-      <c r="A20" s="8" t="s">
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="9" t="s">
         <v>200</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="21" s="13" spans="1:2">
-      <c r="A21" s="8" t="s">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="B21" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="22" s="13" spans="1:2">
-      <c r="A22" s="8" t="s">
+      <c r="B21" s="9"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="9" t="s">
         <v>202</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="23" s="13" spans="1:2">
-      <c r="A23" s="8" t="s">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="B23" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="24" s="13" spans="1:2">
-      <c r="A24" s="8" t="s">
+      <c r="B23" s="9"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="9" t="s">
         <v>204</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="25" s="13" spans="1:2">
-      <c r="A25" s="8" t="s">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="B25" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="26" s="13" spans="1:2">
-      <c r="A26" s="8" t="s">
+      <c r="B25" s="9"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="9" t="s">
         <v>206</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="27" s="13" spans="1:2">
-      <c r="A27" s="8" t="s">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="B27" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="28" s="13" spans="1:2">
-      <c r="A28" s="8" t="s">
+      <c r="B27" s="9"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="9" t="s">
         <v>208</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="29" s="13" spans="1:2">
-      <c r="A29" s="8" t="s">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="B29" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="30" s="13" spans="1:2">
-      <c r="A30" s="8" t="s">
+      <c r="B29" s="9"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="9" t="s">
         <v>210</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="31" s="13" spans="1:2">
-      <c r="A31" s="8" t="s">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="B31" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="32" s="13" spans="1:2">
-      <c r="A32" s="8" t="s">
+      <c r="B31" s="9"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="9" t="s">
         <v>212</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="33" s="13" spans="1:2">
-      <c r="A33" s="8" t="s">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="B33" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="34" s="13" spans="1:2">
-      <c r="A34" s="9" t="s">
+      <c r="B33" s="9"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="9" t="s">
         <v>214</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="35" s="13" spans="1:2">
-      <c r="A35" s="9" t="s">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="B35" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="36" s="13" spans="1:2">
-      <c r="A36" s="9" t="s">
+      <c r="B35" s="9"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="9" t="s">
         <v>216</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="37" s="13" spans="1:2">
-      <c r="A37" s="9" t="s">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="B37" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="38" s="13" spans="1:2">
-      <c r="A38" s="8" t="s">
+      <c r="B37" s="9"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="9" t="s">
         <v>218</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="39" s="13" spans="1:2">
-      <c r="A39" s="8" t="s">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="B39" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="40" s="13" spans="1:2">
-      <c r="A40" s="8" t="s">
+      <c r="B39" s="9"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="9" t="s">
         <v>220</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="41" s="13" spans="1:2">
-      <c r="A41" s="8" t="s">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="B41" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="42" s="13" spans="1:2">
-      <c r="A42" s="8" t="s">
+      <c r="B41" s="9"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="9" t="s">
         <v>222</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="43" s="13" spans="1:2">
-      <c r="A43" s="8" t="s">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="B43" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="44" s="13" spans="1:2">
-      <c r="A44" s="8" t="s">
+      <c r="B43" s="9"/>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="9" t="s">
         <v>224</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="45" s="13" spans="1:2">
-      <c r="A45" s="8" t="s">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="B45" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="46" s="13" spans="1:2">
-      <c r="A46" s="8" t="s">
+      <c r="B45" s="9"/>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="B46" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="47" s="13" spans="1:2">
-      <c r="A47" s="8" t="s">
+      <c r="B46" s="9"/>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="B47" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="48" s="13" spans="1:2">
-      <c r="A48" s="8" t="s">
+      <c r="B47" s="9"/>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="9" t="s">
         <v>228</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="49" s="13" spans="1:2">
-      <c r="A49" s="8" t="s">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="B49" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="50" s="13" spans="1:2">
-      <c r="A50" s="8" t="s">
+      <c r="B49" s="9"/>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="9" t="s">
         <v>230</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="51" s="13" spans="1:2">
-      <c r="A51" s="8" t="s">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="B51" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="52" s="13" spans="1:2">
-      <c r="A52" s="8" t="s">
+      <c r="B51" s="9"/>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="B52" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="53" s="13" spans="1:2">
-      <c r="A53" s="8" t="s">
+      <c r="B52" s="9"/>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="9" t="s">
         <v>233</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="54" s="13" spans="1:2">
-      <c r="A54" s="8" t="s">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B54" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="55" s="13" spans="1:2">
-      <c r="A55" s="8" t="s">
+      <c r="B54" s="9"/>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="9" t="s">
         <v>235</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="56" s="13" spans="1:2">
-      <c r="A56" s="8" t="s">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B56" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="57" s="13" spans="1:2">
-      <c r="A57" s="8" t="s">
+      <c r="B56" s="9"/>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="9" t="s">
         <v>237</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="58" s="13" spans="1:2">
-      <c r="A58" s="8" t="s">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="B58" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="59" s="13" spans="1:2">
-      <c r="A59" s="8" t="s">
+      <c r="B58" s="9"/>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" s="9" t="s">
         <v>239</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="60" s="13" spans="1:2">
-      <c r="A60" s="8" t="s">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="B60" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="61" s="13" spans="1:2">
-      <c r="A61" s="8" t="s">
+      <c r="B60" s="9"/>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="B61" s="9" t="s">
         <v>241</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="62" s="13" spans="1:2">
-      <c r="A62" s="8" t="s">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="B62" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="63" s="13" spans="1:2">
-      <c r="A63" s="8" t="s">
+      <c r="B62" s="9"/>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="B63" s="8" t="s">
+      <c r="B63" s="9" t="s">
         <v>241</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="64" s="13" spans="1:2">
-      <c r="A64" s="8" t="s">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="B64" s="8" t="n"/>
+      <c r="B64" s="9"/>
     </row>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A6" activeCellId="0" pane="topLeft" sqref="A6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="35"/>
-    <col customWidth="1" max="2" min="2" style="1" width="54.2793522267206"/>
-    <col customWidth="1" max="1025" min="3" style="1" width="8.570850202429151"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="54.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="13" spans="1:2">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>181</v>
       </c>
@@ -3117,97 +2941,100 @@
         <v>182</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="2" s="13" spans="1:2">
-      <c r="A2" s="9" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="B2" s="8" t="n"/>
-    </row>
-    <row customHeight="1" ht="15" r="3" s="13" spans="1:2">
-      <c r="A3" s="9" t="s">
+      <c r="B2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>216</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H2" activeCellId="0" pane="topLeft" sqref="H2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="16.8542510121458"/>
-    <col customWidth="1" max="2" min="2" style="1" width="16.5668016194332"/>
-    <col customWidth="1" max="4" min="3" style="1" width="16.8542510121458"/>
-    <col customWidth="1" max="5" min="5" style="1" width="17.2834008097166"/>
-    <col customWidth="1" max="6" min="6" style="1" width="16.5668016194332"/>
-    <col customWidth="1" max="7" min="7" style="1" width="18.2834008097166"/>
-    <col customWidth="1" max="8" min="8" style="1" width="16.5668016194332"/>
-    <col customWidth="1" max="9" min="9" style="1" width="16.8542510121458"/>
-    <col customWidth="1" max="10" min="10" style="1" width="16.5668016194332"/>
-    <col customWidth="1" max="12" min="11" style="1" width="17.5668016194332"/>
-    <col customWidth="1" max="1025" min="13" style="1" width="8.570850202429151"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="16.8542510121458"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.5668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.2834008097166"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.5668016194332"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.8542510121458"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.5668016194332"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="13" spans="1:12">
-      <c r="A1" s="10" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="13" t="s">
         <v>252</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="2" s="13" spans="1:12">
-      <c r="A2" s="8" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>135</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -3222,30 +3049,30 @@
       <c r="F2" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="8" t="s">
         <v>99</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="3" s="13" spans="1:12">
-      <c r="A3" s="8" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>138</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -3254,36 +3081,36 @@
       <c r="D3" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="4" s="13" spans="1:12">
-      <c r="A4" s="8" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>141</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -3292,36 +3119,36 @@
       <c r="D4" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="8" t="s">
         <v>101</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="7" t="s">
         <v>141</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="5" s="13" spans="1:12">
-      <c r="A5" s="8" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>144</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -3330,36 +3157,36 @@
       <c r="D5" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="8" t="s">
         <v>102</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="7" t="s">
         <v>144</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="6" s="13" spans="1:12">
-      <c r="A6" s="8" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>140</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -3368,36 +3195,36 @@
       <c r="D6" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="8" t="s">
         <v>103</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="9" t="s">
         <v>140</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="7" s="13" spans="1:12">
-      <c r="A7" s="8" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>143</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -3406,36 +3233,36 @@
       <c r="D7" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="8" s="13" spans="1:12">
-      <c r="A8" s="8" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>147</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -3444,36 +3271,36 @@
       <c r="D8" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L8" s="7" t="s">
         <v>147</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="9" s="13" spans="1:12">
-      <c r="A9" s="8" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>151</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -3482,36 +3309,36 @@
       <c r="D9" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="K9" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="L9" s="7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="10" s="13" spans="1:12">
-      <c r="A10" s="8" t="s">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>154</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -3520,36 +3347,36 @@
       <c r="D10" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="K10" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="7" t="s">
         <v>154</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="11" s="13" spans="1:12">
-      <c r="A11" s="8" t="s">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>146</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -3558,36 +3385,36 @@
       <c r="D11" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J11" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="L11" s="8" t="s">
+      <c r="L11" s="9" t="s">
         <v>146</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="12" s="13" spans="1:12">
-      <c r="A12" s="8" t="s">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="9" t="s">
         <v>157</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -3596,840 +3423,844 @@
       <c r="D12" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="8" t="s">
         <v>109</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="K12" s="6" t="s">
+      <c r="K12" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="L12" s="6" t="s">
+      <c r="L12" s="7" t="s">
         <v>157</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="13" s="13" spans="1:12">
-      <c r="A13" s="8" t="s">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="K13" s="6" t="s">
+      <c r="K13" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="L13" s="6" t="s">
+      <c r="L13" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="14" s="13" spans="1:12">
-      <c r="A14" s="8" t="s">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="K14" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="L14" s="6" t="s">
+      <c r="L14" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="15" s="13" spans="1:12">
-      <c r="A15" s="8" t="s">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="J15" s="8" t="s">
+      <c r="J15" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="K15" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="L15" s="8" t="s">
+      <c r="L15" s="9" t="s">
         <v>150</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="16" s="13" spans="1:12">
-      <c r="A16" s="8" t="s">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="K16" s="6" t="s">
+      <c r="K16" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="L16" s="6" t="s">
+      <c r="L16" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="17" s="13" spans="1:12">
-      <c r="A17" s="8" t="s">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="J17" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="K17" s="8" t="s">
+      <c r="K17" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="L17" s="8" t="s">
+      <c r="L17" s="9" t="s">
         <v>284</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="18" s="13" spans="1:12">
-      <c r="A18" s="8" t="s">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="J18" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="K18" s="8" t="s">
+      <c r="K18" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="L18" s="8" t="s">
+      <c r="L18" s="9" t="s">
         <v>288</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="19" s="13" spans="1:12">
-      <c r="A19" s="8" t="s">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J19" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="K19" s="6" t="s">
+      <c r="K19" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="L19" s="6" t="s">
+      <c r="L19" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="20" s="13" spans="1:12">
-      <c r="A20" s="8" t="s">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J20" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="K20" s="6" t="s">
+      <c r="K20" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="L20" s="6" t="s">
+      <c r="L20" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="21" s="13" spans="1:12">
-      <c r="A21" s="8" t="s">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="J21" s="8" t="s">
+      <c r="J21" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="K21" s="6" t="s">
+      <c r="K21" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="L21" s="6" t="s">
+      <c r="L21" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="22" s="13" spans="1:12">
-      <c r="A22" s="8" t="s">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I22" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="J22" s="8" t="s">
+      <c r="J22" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="K22" s="6" t="s">
+      <c r="K22" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="L22" s="6" t="s">
+      <c r="L22" s="7" t="s">
         <v>165</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="23" s="13" spans="1:12">
-      <c r="A23" s="8" t="s">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="9" t="s">
         <v>313</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="I23" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="J23" s="8" t="s">
+      <c r="J23" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="K23" s="8" t="s">
+      <c r="K23" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="L23" s="8" t="s">
+      <c r="L23" s="9" t="s">
         <v>313</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="24" s="13" spans="1:12">
-      <c r="A24" s="8" t="s">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="I24" s="6" t="s">
+      <c r="I24" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="J24" s="8" t="s">
+      <c r="J24" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="K24" s="6" t="s">
+      <c r="K24" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="L24" s="6" t="s">
+      <c r="L24" s="7" t="s">
         <v>166</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="25" s="13" spans="1:12">
-      <c r="A25" s="8" t="s">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="I25" s="6" t="s">
+      <c r="I25" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="J25" s="8" t="s">
+      <c r="J25" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="K25" s="6" t="s">
+      <c r="K25" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="L25" s="6" t="s">
+      <c r="L25" s="7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="26" s="13" spans="1:12">
-      <c r="A26" s="8" t="s">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="I26" s="6" t="s">
+      <c r="I26" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="J26" s="8" t="s">
+      <c r="J26" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="K26" s="6" t="s">
+      <c r="K26" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="L26" s="6" t="s">
+      <c r="L26" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="27" s="13" spans="1:12">
-      <c r="A27" s="8" t="s">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="I27" s="6" t="s">
+      <c r="I27" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="J27" s="8" t="s">
+      <c r="J27" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="K27" s="6" t="s">
+      <c r="K27" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="L27" s="6" t="s">
+      <c r="L27" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="28" s="13" spans="1:12">
-      <c r="A28" s="8" t="s">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="I28" s="6" t="s">
+      <c r="I28" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="J28" s="8" t="s">
+      <c r="J28" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="K28" s="6" t="s">
+      <c r="K28" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="L28" s="6" t="s">
+      <c r="L28" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="29" s="13" spans="1:12">
-      <c r="A29" s="8" t="s">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="I29" s="6" t="s">
+      <c r="I29" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="J29" s="8" t="s">
+      <c r="J29" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="K29" s="6" t="s">
+      <c r="K29" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="L29" s="6" t="s">
+      <c r="L29" s="7" t="s">
         <v>171</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="30" s="13" spans="1:12">
-      <c r="A30" s="8" t="s">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="I30" s="6" t="s">
+      <c r="I30" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="J30" s="8" t="s">
+      <c r="J30" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="K30" s="6" t="s">
+      <c r="K30" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L30" s="6" t="s">
+      <c r="L30" s="7" t="s">
         <v>172</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="31" s="13" spans="1:12">
-      <c r="A31" s="8" t="s">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="I31" s="6" t="s">
+      <c r="I31" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="J31" s="8" t="s">
+      <c r="J31" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="K31" s="6" t="s">
+      <c r="K31" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="L31" s="6" t="s">
+      <c r="L31" s="7" t="s">
         <v>173</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="32" s="13" spans="1:12">
-      <c r="A32" s="8" t="s">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="9" t="s">
         <v>323</v>
       </c>
-      <c r="I32" s="6" t="s">
+      <c r="I32" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J32" s="8" t="s">
+      <c r="J32" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="K32" s="8" t="s">
+      <c r="K32" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="L32" s="8" t="s">
+      <c r="L32" s="9" t="s">
         <v>159</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="33" s="13" spans="1:12">
-      <c r="A33" s="8" t="s">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="I33" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="J33" s="8" t="s">
+      <c r="J33" s="9" t="s">
         <v>323</v>
       </c>
-      <c r="K33" s="6" t="s">
+      <c r="K33" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="L33" s="6" t="s">
+      <c r="L33" s="7" t="s">
         <v>174</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="34" s="13" spans="1:12">
-      <c r="A34" s="8" t="s">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="I34" s="6" t="s">
+      <c r="I34" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="J34" s="8" t="s">
+      <c r="J34" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="K34" s="6" t="s">
+      <c r="K34" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="L34" s="6" t="s">
+      <c r="L34" s="7" t="s">
         <v>175</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="35" s="13" spans="1:12">
-      <c r="A35" s="8" t="s">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="I35" s="6" t="s">
+      <c r="I35" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="J35" s="8" t="s">
+      <c r="J35" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="K35" s="6" t="s">
+      <c r="K35" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="L35" s="6" t="s">
+      <c r="L35" s="7" t="s">
         <v>176</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="36" s="13" spans="1:12">
-      <c r="A36" s="8" t="s">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="K36" s="6" t="s">
+      <c r="K36" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="L36" s="6" t="s">
+      <c r="L36" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="37" s="13" spans="1:12">
-      <c r="A37" s="8" t="s">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="K37" s="6" t="s">
+      <c r="K37" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="L37" s="6" t="s">
+      <c r="L37" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="38" s="13" spans="1:12">
-      <c r="A38" s="8" t="s">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="K38" s="6" t="s">
+      <c r="K38" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="L38" s="6" t="s">
+      <c r="L38" s="7" t="s">
         <v>179</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="39" s="13" spans="1:12">
-      <c r="A39" s="8" t="s">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="K39" s="6" t="s">
+      <c r="K39" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="L39" s="6" t="s">
+      <c r="L39" s="7" t="s">
         <v>180</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="40" s="13" spans="1:12">
-      <c r="A40" s="8" t="s">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="K40" s="8" t="s">
+      <c r="K40" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="L40" s="8" t="s">
+      <c r="L40" s="9" t="s">
         <v>174</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="41" s="13" spans="1:12">
-      <c r="A41" s="8" t="s">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="K41" s="8" t="s">
+      <c r="K41" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="L41" s="8" t="s">
+      <c r="L41" s="9" t="s">
         <v>168</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="42" s="13" spans="1:12">
-      <c r="A42" s="8" t="n"/>
-      <c r="B42" s="8" t="n"/>
-      <c r="C42" s="8" t="s">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="9" t="s">
         <v>152</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="43" s="13" spans="1:12">
-      <c r="A43" s="8" t="n"/>
-      <c r="B43" s="8" t="n"/>
-      <c r="C43" s="8" t="s">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="9" t="s">
         <v>285</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="44" s="13" spans="1:12">
-      <c r="A44" s="8" t="n"/>
-      <c r="B44" s="8" t="n"/>
-      <c r="C44" s="8" t="s">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="9" t="s">
         <v>321</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="45" s="13" spans="1:12">
-      <c r="A45" s="8" t="n"/>
-      <c r="B45" s="8" t="n"/>
-      <c r="C45" s="8" t="s">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="9" t="s">
         <v>303</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="46" s="13" spans="1:12">
-      <c r="A46" s="8" t="n"/>
-      <c r="B46" s="8" t="n"/>
-      <c r="C46" s="8" t="s">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="9" t="s">
         <v>282</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="47" s="13" spans="1:12">
-      <c r="A47" s="8" t="n"/>
-      <c r="B47" s="8" t="n"/>
-      <c r="C47" s="8" t="s">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="9" t="s">
         <v>299</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="48" s="13" spans="1:12">
-      <c r="A48" s="8" t="n"/>
-      <c r="B48" s="8" t="n"/>
-      <c r="C48" s="8" t="s">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="9" t="s">
         <v>305</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="49" s="13" spans="1:12">
-      <c r="A49" s="8" t="n"/>
-      <c r="B49" s="8" t="n"/>
-      <c r="C49" s="8" t="s">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="9" t="s">
         <v>155</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="50" s="13" spans="1:12">
-      <c r="A50" s="8" t="n"/>
-      <c r="B50" s="8" t="n"/>
-      <c r="C50" s="8" t="s">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D50" s="9" t="s">
         <v>325</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="51" s="13" spans="1:12">
-      <c r="A51" s="8" t="n"/>
-      <c r="B51" s="8" t="n"/>
-      <c r="C51" s="8" t="s">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D51" s="9" t="s">
         <v>294</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>